<commit_message>
Update automatico via Actualizar 05-06-2020 21-48-23
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{965BA304-47E0-4BCA-83F7-0599D113EC0E}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B5969E97-5243-4910-BAF5-D019EC74BF8D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="246">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -156,6 +156,9 @@
     <t>Piedra Pintada o La Colorada</t>
   </si>
   <si>
+    <t>centro de salud</t>
+  </si>
+  <si>
     <t>CESAMO Corozal</t>
   </si>
   <si>
@@ -177,10 +180,10 @@
     <t>Clínica De Especialdades</t>
   </si>
   <si>
-    <t>Emergencias Medicas</t>
-  </si>
-  <si>
-    <t>Clínica médica Edgar Padilla</t>
+    <t>Emergencias Médicas</t>
+  </si>
+  <si>
+    <t>Clínica Médica Edgar Padilla</t>
   </si>
   <si>
     <t>04</t>
@@ -243,7 +246,7 @@
     <t>HND-0506</t>
   </si>
   <si>
-    <t>Cruz Roja Hondureña, Puerto Cortés</t>
+    <t>Cruz Roja Hondureña</t>
   </si>
   <si>
     <t>06</t>
@@ -261,7 +264,7 @@
     <t>HND-0601</t>
   </si>
   <si>
-    <t>San Francisco de Asís</t>
+    <t>Clínica San Francisco de Asís</t>
   </si>
   <si>
     <t>Ashonplafa</t>
@@ -309,7 +312,7 @@
     <t>Laboratorio y Droguería Francelia</t>
   </si>
   <si>
-    <t>Clíper Hato de Enmedio</t>
+    <t>Clínica Clíper Hato de Enmedio</t>
   </si>
   <si>
     <t>Asociación Pediatrica Hondureña</t>
@@ -336,10 +339,7 @@
     <t>Clínica Rivera</t>
   </si>
   <si>
-    <t>Clínicas Viera</t>
-  </si>
-  <si>
-    <t>Viera</t>
+    <t>Hospital y Clínicas Viera</t>
   </si>
   <si>
     <t>Clínica Salesiano</t>
@@ -393,9 +393,6 @@
     <t>HND-1007</t>
   </si>
   <si>
-    <t>Cruz roja Hondureña</t>
-  </si>
-  <si>
     <t>Centro de Salud Camilo Giron Rivera</t>
   </si>
   <si>
@@ -438,7 +435,7 @@
     <t>HND-1311</t>
   </si>
   <si>
-    <t>CLINICA MEDICA VIDA ABUNDANTE</t>
+    <t>Clínica Médica Vida Abundante</t>
   </si>
   <si>
     <t>15</t>
@@ -459,7 +456,7 @@
     <t>HND-1505</t>
   </si>
   <si>
-    <t>CLÍNICA SINAÍ</t>
+    <t>Clínica Sinaí</t>
   </si>
   <si>
     <t>18</t>
@@ -480,7 +477,7 @@
     <t>HND-1804</t>
   </si>
   <si>
-    <t>clínica del ojo</t>
+    <t>Clínica del Ojo</t>
   </si>
   <si>
     <t>1806</t>
@@ -495,7 +492,7 @@
     <t>HND-1806</t>
   </si>
   <si>
-    <t>Pliclinica San Jorge</t>
+    <t>Policlínica San Jorge</t>
   </si>
   <si>
     <t>Atlantida</t>
@@ -567,10 +564,7 @@
     <t>HND-0404</t>
   </si>
   <si>
-    <t>Cruz Roja</t>
-  </si>
-  <si>
-    <t>Hospital Leonardo Martinez</t>
+    <t>Hospital Leonardo Martínez</t>
   </si>
   <si>
     <t>Hospital Bendaña</t>
@@ -582,13 +576,13 @@
     <t>Centro de Diagnóstico Clínico</t>
   </si>
   <si>
-    <t>Clínica San Jorge</t>
+    <t>Hospital San Jorge</t>
   </si>
   <si>
     <t>Hospital del Niño</t>
   </si>
   <si>
-    <t>Centro Medico</t>
+    <t>Centro Médico</t>
   </si>
   <si>
     <t>DIME</t>
@@ -597,10 +591,7 @@
     <t>Clínica Santa Lucia</t>
   </si>
   <si>
-    <t>Laboratorios Clinicos express</t>
-  </si>
-  <si>
-    <t>Cruz Roja Hondureña</t>
+    <t>Laboratorios Clínicos Express</t>
   </si>
   <si>
     <t>La Policlínica</t>
@@ -612,7 +603,7 @@
     <t>Instituto Nacional Cardiopulmonar</t>
   </si>
   <si>
-    <t>Centro de Salud el Manchen</t>
+    <t>Centro de Salud El Manchen</t>
   </si>
   <si>
     <t>Centro Salud Sagrada Familia</t>
@@ -624,7 +615,7 @@
     <t>Clínica Fudena</t>
   </si>
   <si>
-    <t>Centor de Salud El Chile</t>
+    <t>Centro de Salud El Chile</t>
   </si>
   <si>
     <t>Centro de Salud El Bosque</t>
@@ -1754,8 +1745,8 @@
   <dimension ref="A1:W83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="P2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -1770,7 +1761,7 @@
     <col min="8" max="8" width="17.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="15.28515625" style="1" customWidth="1"/>
@@ -1979,10 +1970,10 @@
         <v>35</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V3" s="2">
         <v>14.159800000000001</v>
@@ -2020,10 +2011,10 @@
         <v>5</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>30</v>
@@ -2032,16 +2023,16 @@
         <v>14</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>35</v>
@@ -2050,7 +2041,7 @@
         <v>36</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="V4" s="2">
         <v>14.068899999999999</v>
@@ -2088,10 +2079,10 @@
         <v>5</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>30</v>
@@ -2100,16 +2091,16 @@
         <v>14</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>35</v>
@@ -2118,7 +2109,7 @@
         <v>36</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="V5" s="2">
         <v>14.0501</v>
@@ -2156,10 +2147,10 @@
         <v>5</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>30</v>
@@ -2168,16 +2159,16 @@
         <v>14</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>35</v>
@@ -2186,7 +2177,7 @@
         <v>36</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="V6" s="2">
         <v>14.3118</v>
@@ -2212,10 +2203,10 @@
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>27</v>
@@ -2224,10 +2215,10 @@
         <v>2</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>30</v>
@@ -2236,16 +2227,16 @@
         <v>1</v>
       </c>
       <c r="N7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="P7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>35</v>
@@ -2254,7 +2245,7 @@
         <v>36</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="V7" s="2">
         <v>14.3165</v>
@@ -2280,10 +2271,10 @@
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>27</v>
@@ -2292,10 +2283,10 @@
         <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>30</v>
@@ -2304,16 +2295,16 @@
         <v>1</v>
       </c>
       <c r="N8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="P8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>35</v>
@@ -2322,7 +2313,7 @@
         <v>36</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="V8" s="2">
         <v>14.2385</v>
@@ -2348,10 +2339,10 @@
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>27</v>
@@ -2360,10 +2351,10 @@
         <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>30</v>
@@ -2372,16 +2363,16 @@
         <v>1</v>
       </c>
       <c r="N9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="P9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>35</v>
@@ -2390,7 +2381,7 @@
         <v>36</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="V9" s="2">
         <v>14.239100000000001</v>
@@ -2416,10 +2407,10 @@
         <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>27</v>
@@ -2428,10 +2419,10 @@
         <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>30</v>
@@ -2440,16 +2431,16 @@
         <v>1</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="P10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>35</v>
@@ -2458,7 +2449,7 @@
         <v>36</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="V10" s="2">
         <v>14.244999999999999</v>
@@ -2484,10 +2475,10 @@
         <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>27</v>
@@ -2496,10 +2487,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>30</v>
@@ -2508,16 +2499,16 @@
         <v>1</v>
       </c>
       <c r="N11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="P11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>35</v>
@@ -2526,7 +2517,7 @@
         <v>36</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="V11" s="2">
         <v>14.245100000000001</v>
@@ -2552,10 +2543,10 @@
         <v>5</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>27</v>
@@ -2564,10 +2555,10 @@
         <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>30</v>
@@ -2576,16 +2567,16 @@
         <v>1</v>
       </c>
       <c r="N12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="P12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>35</v>
@@ -2594,7 +2585,7 @@
         <v>36</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="V12" s="2">
         <v>14.246</v>
@@ -2620,10 +2611,10 @@
         <v>5</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>27</v>
@@ -2632,10 +2623,10 @@
         <v>6</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>30</v>
@@ -2644,16 +2635,16 @@
         <v>1</v>
       </c>
       <c r="N13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="P13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>35</v>
@@ -2662,7 +2653,7 @@
         <v>36</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="V13" s="2">
         <v>14.579700000000001</v>
@@ -2688,10 +2679,10 @@
         <v>6</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>27</v>
@@ -2700,11 +2691,11 @@
         <v>1</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="L14" s="1" t="s">
         <v>30</v>
       </c>
@@ -2712,16 +2703,16 @@
         <v>1</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>35</v>
@@ -2730,7 +2721,7 @@
         <v>36</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V14" s="2">
         <v>14.5837</v>
@@ -2756,10 +2747,10 @@
         <v>6</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>27</v>
@@ -2768,11 +2759,11 @@
         <v>1</v>
       </c>
       <c r="J15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="L15" s="1" t="s">
         <v>30</v>
       </c>
@@ -2780,16 +2771,16 @@
         <v>1</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>35</v>
@@ -2798,7 +2789,7 @@
         <v>36</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="V15" s="2">
         <v>14.5839</v>
@@ -2824,10 +2815,10 @@
         <v>6</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>27</v>
@@ -2836,11 +2827,11 @@
         <v>1</v>
       </c>
       <c r="J16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="L16" s="1" t="s">
         <v>30</v>
       </c>
@@ -2848,16 +2839,16 @@
         <v>1</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>35</v>
@@ -2866,7 +2857,7 @@
         <v>36</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="V16" s="2">
         <v>14.5844</v>
@@ -2892,10 +2883,10 @@
         <v>6</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>27</v>
@@ -2904,10 +2895,10 @@
         <v>6</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>30</v>
@@ -2916,16 +2907,16 @@
         <v>3</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R17" s="1" t="s">
         <v>35</v>
@@ -2934,7 +2925,7 @@
         <v>36</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="V17" s="2">
         <v>14.5852</v>
@@ -2960,10 +2951,10 @@
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>27</v>
@@ -2972,10 +2963,10 @@
         <v>1</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>30</v>
@@ -2984,16 +2975,16 @@
         <v>1</v>
       </c>
       <c r="N18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O18" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>35</v>
@@ -3002,7 +2993,7 @@
         <v>36</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="V18" s="2">
         <v>14.5854</v>
@@ -3028,10 +3019,10 @@
         <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>27</v>
@@ -3040,10 +3031,10 @@
         <v>1</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>30</v>
@@ -3052,16 +3043,16 @@
         <v>1</v>
       </c>
       <c r="N19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O19" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P19" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R19" s="1" t="s">
         <v>35</v>
@@ -3070,7 +3061,7 @@
         <v>36</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="V19" s="2">
         <v>14.5855</v>
@@ -3096,10 +3087,10 @@
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>27</v>
@@ -3108,10 +3099,10 @@
         <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>30</v>
@@ -3120,16 +3111,16 @@
         <v>1</v>
       </c>
       <c r="N20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O20" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O20" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R20" s="1" t="s">
         <v>35</v>
@@ -3138,7 +3129,7 @@
         <v>36</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="V20" s="2">
         <v>14.585699999999999</v>
@@ -3164,10 +3155,10 @@
         <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>27</v>
@@ -3176,10 +3167,10 @@
         <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>30</v>
@@ -3188,16 +3179,16 @@
         <v>1</v>
       </c>
       <c r="N21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P21" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R21" s="1" t="s">
         <v>35</v>
@@ -3206,7 +3197,7 @@
         <v>36</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="V21" s="2">
         <v>14.585699999999999</v>
@@ -3232,10 +3223,10 @@
         <v>8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>27</v>
@@ -3244,10 +3235,10 @@
         <v>1</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>30</v>
@@ -3256,25 +3247,25 @@
         <v>1</v>
       </c>
       <c r="N22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O22" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R22" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="V22" s="2">
         <v>14.585800000000001</v>
@@ -3300,10 +3291,10 @@
         <v>8</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>27</v>
@@ -3312,10 +3303,10 @@
         <v>1</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>30</v>
@@ -3324,16 +3315,16 @@
         <v>1</v>
       </c>
       <c r="N23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O23" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P23" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R23" s="1" t="s">
         <v>35</v>
@@ -3342,7 +3333,7 @@
         <v>36</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="V23" s="2">
         <v>14.585900000000001</v>
@@ -3368,10 +3359,10 @@
         <v>8</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>27</v>
@@ -3380,10 +3371,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>30</v>
@@ -3392,16 +3383,16 @@
         <v>1</v>
       </c>
       <c r="N24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O24" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P24" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R24" s="1" t="s">
         <v>35</v>
@@ -3410,7 +3401,7 @@
         <v>36</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="V24" s="2">
         <v>14.585900000000001</v>
@@ -3436,10 +3427,10 @@
         <v>8</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>27</v>
@@ -3448,10 +3439,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>30</v>
@@ -3460,16 +3451,16 @@
         <v>1</v>
       </c>
       <c r="N25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O25" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P25" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R25" s="1" t="s">
         <v>35</v>
@@ -3478,7 +3469,7 @@
         <v>36</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="V25" s="2">
         <v>14.5862</v>
@@ -3504,10 +3495,10 @@
         <v>8</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>27</v>
@@ -3516,10 +3507,10 @@
         <v>1</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>30</v>
@@ -3528,16 +3519,16 @@
         <v>1</v>
       </c>
       <c r="N26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O26" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P26" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R26" s="1" t="s">
         <v>35</v>
@@ -3546,7 +3537,7 @@
         <v>36</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="V26" s="2">
         <v>14.5869</v>
@@ -3572,10 +3563,10 @@
         <v>8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>27</v>
@@ -3584,10 +3575,10 @@
         <v>1</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>30</v>
@@ -3596,16 +3587,16 @@
         <v>1</v>
       </c>
       <c r="N27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O27" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P27" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R27" s="1" t="s">
         <v>35</v>
@@ -3614,7 +3605,7 @@
         <v>36</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="V27" s="2">
         <v>14.587300000000001</v>
@@ -3640,10 +3631,10 @@
         <v>8</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>27</v>
@@ -3652,10 +3643,10 @@
         <v>1</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>30</v>
@@ -3664,16 +3655,16 @@
         <v>1</v>
       </c>
       <c r="N28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O28" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P28" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R28" s="1" t="s">
         <v>35</v>
@@ -3682,7 +3673,7 @@
         <v>36</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="V28" s="2">
         <v>14.5875</v>
@@ -3708,10 +3699,10 @@
         <v>8</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>27</v>
@@ -3720,10 +3711,10 @@
         <v>1</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>30</v>
@@ -3732,16 +3723,16 @@
         <v>1</v>
       </c>
       <c r="N29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O29" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O29" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R29" s="1" t="s">
         <v>35</v>
@@ -3750,7 +3741,7 @@
         <v>36</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="V29" s="2">
         <v>14.5877</v>
@@ -3776,10 +3767,10 @@
         <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>27</v>
@@ -3788,10 +3779,10 @@
         <v>1</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>30</v>
@@ -3800,16 +3791,16 @@
         <v>1</v>
       </c>
       <c r="N30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O30" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P30" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R30" s="1" t="s">
         <v>35</v>
@@ -3844,10 +3835,10 @@
         <v>8</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>27</v>
@@ -3856,10 +3847,10 @@
         <v>1</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>30</v>
@@ -3868,16 +3859,16 @@
         <v>1</v>
       </c>
       <c r="N31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O31" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P31" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R31" s="1" t="s">
         <v>35</v>
@@ -3912,10 +3903,10 @@
         <v>8</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>27</v>
@@ -3924,10 +3915,10 @@
         <v>1</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>30</v>
@@ -3945,7 +3936,7 @@
         <v>33</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R32" s="1" t="s">
         <v>35</v>
@@ -3980,10 +3971,10 @@
         <v>8</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>27</v>
@@ -4048,10 +4039,10 @@
         <v>8</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>27</v>
@@ -4116,10 +4107,10 @@
         <v>8</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>27</v>
@@ -4226,7 +4217,7 @@
         <v>36</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="V36" s="2">
         <v>14.5885</v>
@@ -4294,7 +4285,7 @@
         <v>36</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="V37" s="2">
         <v>14.5886</v>
@@ -4362,7 +4353,7 @@
         <v>36</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V38" s="2">
         <v>14.5886</v>
@@ -4430,7 +4421,7 @@
         <v>36</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V39" s="2">
         <v>14.588699999999999</v>
@@ -4456,40 +4447,40 @@
         <v>13</v>
       </c>
       <c r="F40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I40" s="1">
+        <v>1</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I40" s="1">
-        <v>1</v>
-      </c>
-      <c r="J40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M40" s="1">
+        <v>1</v>
+      </c>
+      <c r="N40" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M40" s="1">
-        <v>1</v>
-      </c>
-      <c r="N40" s="1" t="s">
+      <c r="O40" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q40" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="R40" s="1" t="s">
         <v>35</v>
@@ -4498,7 +4489,7 @@
         <v>36</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="V40" s="2">
         <v>14.588699999999999</v>
@@ -4524,10 +4515,10 @@
         <v>13</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>27</v>
@@ -4536,28 +4527,28 @@
         <v>11</v>
       </c>
       <c r="J41" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K41" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M41" s="1">
+        <v>1</v>
+      </c>
+      <c r="N41" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M41" s="1">
-        <v>1</v>
-      </c>
-      <c r="N41" s="1" t="s">
+      <c r="O41" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q41" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="R41" s="1" t="s">
         <v>35</v>
@@ -4566,7 +4557,7 @@
         <v>36</v>
       </c>
       <c r="U41" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="V41" s="2">
         <v>14.588800000000001</v>
@@ -4592,10 +4583,10 @@
         <v>15</v>
       </c>
       <c r="F42" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>27</v>
@@ -4604,28 +4595,28 @@
         <v>5</v>
       </c>
       <c r="J42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K42" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="L42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M42" s="1">
+        <v>1</v>
+      </c>
+      <c r="N42" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="L42" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M42" s="1">
-        <v>1</v>
-      </c>
-      <c r="N42" s="1" t="s">
+      <c r="O42" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q42" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="R42" s="1" t="s">
         <v>35</v>
@@ -4634,7 +4625,7 @@
         <v>36</v>
       </c>
       <c r="U42" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="V42" s="2">
         <v>14.588800000000001</v>
@@ -4660,10 +4651,10 @@
         <v>18</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>27</v>
@@ -4672,28 +4663,28 @@
         <v>4</v>
       </c>
       <c r="J43" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K43" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="L43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M43" s="1">
+        <v>1</v>
+      </c>
+      <c r="N43" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="L43" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M43" s="1">
-        <v>1</v>
-      </c>
-      <c r="N43" s="1" t="s">
+      <c r="O43" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q43" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="R43" s="1" t="s">
         <v>35</v>
@@ -4702,7 +4693,7 @@
         <v>36</v>
       </c>
       <c r="U43" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V43" s="2">
         <v>14.588900000000001</v>
@@ -4728,10 +4719,10 @@
         <v>18</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>27</v>
@@ -4740,28 +4731,28 @@
         <v>6</v>
       </c>
       <c r="J44" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K44" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="L44" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M44" s="1">
+        <v>1</v>
+      </c>
+      <c r="N44" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M44" s="1">
-        <v>1</v>
-      </c>
-      <c r="N44" s="1" t="s">
+      <c r="O44" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q44" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q44" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="R44" s="1" t="s">
         <v>35</v>
@@ -4770,7 +4761,7 @@
         <v>36</v>
       </c>
       <c r="U44" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="V44" s="2">
         <v>14.588900000000001</v>
@@ -4799,7 +4790,7 @@
         <v>25</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>27</v>
@@ -4820,7 +4811,7 @@
         <v>1</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O45" s="1" t="s">
         <v>29</v>
@@ -4835,10 +4826,10 @@
         <v>35</v>
       </c>
       <c r="S45" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="U45" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="U45" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="V45" s="2">
         <v>15.399699999999999</v>
@@ -4867,7 +4858,7 @@
         <v>25</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>27</v>
@@ -4876,10 +4867,10 @@
         <v>5</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>30</v>
@@ -4888,25 +4879,25 @@
         <v>14</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P46" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R46" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
       <c r="U46" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="V46" s="2">
         <v>15.399800000000001</v>
@@ -4932,10 +4923,10 @@
         <v>2</v>
       </c>
       <c r="F47" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>27</v>
@@ -4944,37 +4935,37 @@
         <v>8</v>
       </c>
       <c r="J47" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K47" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="L47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M47" s="1">
+        <v>1</v>
+      </c>
+      <c r="N47" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L47" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M47" s="1">
-        <v>1</v>
-      </c>
-      <c r="N47" s="1" t="s">
+      <c r="O47" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q47" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="O47" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="P47" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q47" s="1" t="s">
+      <c r="R47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S47" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="U47" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="R47" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S47" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="U47" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="V47" s="2">
         <v>15.399900000000001</v>
@@ -5000,10 +4991,10 @@
         <v>3</v>
       </c>
       <c r="F48" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>27</v>
@@ -5012,37 +5003,37 @@
         <v>18</v>
       </c>
       <c r="J48" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K48" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="L48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M48" s="1">
+        <v>1</v>
+      </c>
+      <c r="N48" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="L48" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M48" s="1">
-        <v>1</v>
-      </c>
-      <c r="N48" s="1" t="s">
+      <c r="O48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q48" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="O48" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q48" s="1" t="s">
+      <c r="R48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S48" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="U48" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="R48" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S48" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="U48" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="V48" s="2">
         <v>15.400499999999999</v>
@@ -5068,10 +5059,10 @@
         <v>4</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>27</v>
@@ -5080,37 +5071,37 @@
         <v>4</v>
       </c>
       <c r="J49" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K49" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="L49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M49" s="1">
+        <v>1</v>
+      </c>
+      <c r="N49" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L49" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M49" s="1">
-        <v>1</v>
-      </c>
-      <c r="N49" s="1" t="s">
+      <c r="O49" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q49" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="O49" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="P49" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q49" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="R49" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S49" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U49" s="1" t="s">
-        <v>177</v>
+        <v>70</v>
       </c>
       <c r="V49" s="2">
         <v>15.400600000000001</v>
@@ -5136,10 +5127,10 @@
         <v>5</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>27</v>
@@ -5148,10 +5139,10 @@
         <v>1</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>30</v>
@@ -5160,25 +5151,25 @@
         <v>1</v>
       </c>
       <c r="N50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O50" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O50" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="P50" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R50" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S50" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U50" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="V50" s="2">
         <v>15.400700000000001</v>
@@ -5204,10 +5195,10 @@
         <v>5</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>27</v>
@@ -5216,10 +5207,10 @@
         <v>1</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>30</v>
@@ -5228,25 +5219,25 @@
         <v>1</v>
       </c>
       <c r="N51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O51" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O51" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="P51" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R51" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U51" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="V51" s="2">
         <v>15.4009</v>
@@ -5272,10 +5263,10 @@
         <v>5</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>27</v>
@@ -5284,10 +5275,10 @@
         <v>1</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>30</v>
@@ -5296,25 +5287,25 @@
         <v>1</v>
       </c>
       <c r="N52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O52" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O52" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="P52" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R52" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S52" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U52" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="V52" s="2">
         <v>15.4009</v>
@@ -5340,10 +5331,10 @@
         <v>5</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>27</v>
@@ -5352,10 +5343,10 @@
         <v>1</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>30</v>
@@ -5364,25 +5355,25 @@
         <v>1</v>
       </c>
       <c r="N53" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O53" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O53" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="P53" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R53" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S53" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U53" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="V53" s="2">
         <v>15.4009</v>
@@ -5408,10 +5399,10 @@
         <v>8</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>27</v>
@@ -5420,10 +5411,10 @@
         <v>1</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>30</v>
@@ -5432,25 +5423,25 @@
         <v>1</v>
       </c>
       <c r="N54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O54" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O54" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P54" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R54" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S54" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U54" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="V54" s="2">
         <v>15.401</v>
@@ -5476,10 +5467,10 @@
         <v>8</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>27</v>
@@ -5488,10 +5479,10 @@
         <v>1</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>30</v>
@@ -5500,25 +5491,25 @@
         <v>1</v>
       </c>
       <c r="N55" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O55" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O55" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P55" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R55" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U55" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="V55" s="2">
         <v>15.401</v>
@@ -5544,10 +5535,10 @@
         <v>8</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>27</v>
@@ -5556,10 +5547,10 @@
         <v>1</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>30</v>
@@ -5568,25 +5559,25 @@
         <v>1</v>
       </c>
       <c r="N56" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O56" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O56" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P56" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R56" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U56" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="V56" s="2">
         <v>15.4011</v>
@@ -5612,10 +5603,10 @@
         <v>8</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>27</v>
@@ -5624,10 +5615,10 @@
         <v>1</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>30</v>
@@ -5636,25 +5627,25 @@
         <v>1</v>
       </c>
       <c r="N57" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O57" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O57" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P57" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R57" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S57" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U57" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="V57" s="2">
         <v>15.4011</v>
@@ -5680,10 +5671,10 @@
         <v>8</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>27</v>
@@ -5692,10 +5683,10 @@
         <v>1</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>30</v>
@@ -5704,25 +5695,25 @@
         <v>1</v>
       </c>
       <c r="N58" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O58" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O58" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P58" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R58" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S58" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U58" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="V58" s="2">
         <v>15.4011</v>
@@ -5748,10 +5739,10 @@
         <v>8</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>27</v>
@@ -5760,10 +5751,10 @@
         <v>1</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>30</v>
@@ -5772,25 +5763,25 @@
         <v>1</v>
       </c>
       <c r="N59" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O59" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O59" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P59" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R59" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S59" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U59" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="V59" s="2">
         <v>15.4011</v>
@@ -5816,10 +5807,10 @@
         <v>8</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>27</v>
@@ -5828,10 +5819,10 @@
         <v>1</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>30</v>
@@ -5840,25 +5831,25 @@
         <v>1</v>
       </c>
       <c r="N60" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O60" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O60" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P60" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R60" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S60" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U60" s="1" t="s">
-        <v>188</v>
+        <v>70</v>
       </c>
       <c r="V60" s="2">
         <v>15.401199999999999</v>
@@ -5884,10 +5875,10 @@
         <v>8</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>27</v>
@@ -5896,10 +5887,10 @@
         <v>1</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L61" s="1" t="s">
         <v>30</v>
@@ -5908,25 +5899,25 @@
         <v>1</v>
       </c>
       <c r="N61" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O61" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O61" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P61" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q61" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R61" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U61" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="V61" s="2">
         <v>15.401300000000001</v>
@@ -5952,10 +5943,10 @@
         <v>8</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>27</v>
@@ -5964,10 +5955,10 @@
         <v>1</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>30</v>
@@ -5976,25 +5967,25 @@
         <v>1</v>
       </c>
       <c r="N62" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O62" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O62" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P62" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R62" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S62" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U62" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="V62" s="2">
         <v>15.401300000000001</v>
@@ -6020,10 +6011,10 @@
         <v>8</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>27</v>
@@ -6032,10 +6023,10 @@
         <v>1</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>30</v>
@@ -6044,25 +6035,25 @@
         <v>1</v>
       </c>
       <c r="N63" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O63" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O63" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P63" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q63" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R63" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S63" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U63" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="V63" s="2">
         <v>15.401400000000001</v>
@@ -6088,10 +6079,10 @@
         <v>8</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>27</v>
@@ -6100,10 +6091,10 @@
         <v>1</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>30</v>
@@ -6112,25 +6103,25 @@
         <v>1</v>
       </c>
       <c r="N64" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O64" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O64" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P64" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q64" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R64" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S64" s="1" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
       <c r="U64" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="V64" s="2">
         <v>15.401400000000001</v>
@@ -6156,10 +6147,10 @@
         <v>8</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>27</v>
@@ -6168,10 +6159,10 @@
         <v>1</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>30</v>
@@ -6180,25 +6171,25 @@
         <v>1</v>
       </c>
       <c r="N65" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O65" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O65" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P65" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q65" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R65" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S65" s="1" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
       <c r="U65" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="V65" s="2">
         <v>15.401400000000001</v>
@@ -6224,10 +6215,10 @@
         <v>8</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>27</v>
@@ -6236,10 +6227,10 @@
         <v>1</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>30</v>
@@ -6248,25 +6239,25 @@
         <v>1</v>
       </c>
       <c r="N66" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O66" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O66" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P66" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q66" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R66" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S66" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U66" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="V66" s="2">
         <v>15.4015</v>
@@ -6292,10 +6283,10 @@
         <v>8</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>27</v>
@@ -6304,10 +6295,10 @@
         <v>1</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>30</v>
@@ -6316,25 +6307,25 @@
         <v>1</v>
       </c>
       <c r="N67" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O67" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O67" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P67" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R67" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S67" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U67" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="V67" s="2">
         <v>15.4015</v>
@@ -6360,10 +6351,10 @@
         <v>8</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>27</v>
@@ -6372,10 +6363,10 @@
         <v>1</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>30</v>
@@ -6384,25 +6375,25 @@
         <v>1</v>
       </c>
       <c r="N68" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O68" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O68" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P68" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R68" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S68" s="1" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
       <c r="U68" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="V68" s="2">
         <v>15.4016</v>
@@ -6428,10 +6419,10 @@
         <v>8</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>27</v>
@@ -6440,10 +6431,10 @@
         <v>1</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L69" s="1" t="s">
         <v>30</v>
@@ -6452,25 +6443,25 @@
         <v>1</v>
       </c>
       <c r="N69" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O69" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O69" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="P69" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R69" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S69" s="1" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
       <c r="U69" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="V69" s="2">
         <v>15.4016</v>
@@ -6496,10 +6487,10 @@
         <v>8</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>27</v>
@@ -6508,37 +6499,37 @@
         <v>26</v>
       </c>
       <c r="J70" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M70" s="1">
+        <v>1</v>
+      </c>
+      <c r="N70" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="O70" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="P70" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q70" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K70" s="1" t="s">
+      <c r="R70" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S70" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="U70" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="L70" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M70" s="1">
-        <v>1</v>
-      </c>
-      <c r="N70" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="O70" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P70" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q70" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="R70" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S70" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="U70" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="V70" s="2">
         <v>15.4016</v>
@@ -6576,7 +6567,7 @@
         <v>6</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>114</v>
@@ -6588,7 +6579,7 @@
         <v>1</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="O71" s="1" t="s">
         <v>114</v>
@@ -6597,16 +6588,16 @@
         <v>33</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="R71" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S71" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U71" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="V71" s="2">
         <v>15.4016</v>
@@ -6644,10 +6635,10 @@
         <v>13</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L72" s="1" t="s">
         <v>30</v>
@@ -6656,25 +6647,25 @@
         <v>4</v>
       </c>
       <c r="N72" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="O72" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="P72" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q72" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="R72" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S72" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="U72" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="O72" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="P72" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q72" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="R72" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S72" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="U72" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="V72" s="2">
         <v>15.4016</v>
@@ -6700,22 +6691,22 @@
         <v>11</v>
       </c>
       <c r="F73" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I73" s="1">
+        <v>1</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="K73" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I73" s="1">
-        <v>1</v>
-      </c>
-      <c r="J73" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="K73" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>30</v>
@@ -6724,25 +6715,25 @@
         <v>7</v>
       </c>
       <c r="N73" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="O73" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="P73" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q73" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="R73" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S73" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="U73" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="O73" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="P73" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q73" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="R73" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S73" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="U73" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="V73" s="2">
         <v>15.4016</v>
@@ -6768,10 +6759,10 @@
         <v>11</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>27</v>
@@ -6780,37 +6771,37 @@
         <v>4</v>
       </c>
       <c r="J74" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M74" s="1">
+        <v>1</v>
+      </c>
+      <c r="N74" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="P74" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q74" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="K74" s="1" t="s">
+      <c r="R74" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S74" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U74" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="L74" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M74" s="1">
-        <v>1</v>
-      </c>
-      <c r="N74" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="O74" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="P74" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q74" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="R74" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S74" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="U74" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="V74" s="2">
         <v>15.4016</v>
@@ -6836,10 +6827,10 @@
         <v>11</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>27</v>
@@ -6848,37 +6839,37 @@
         <v>4</v>
       </c>
       <c r="J75" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M75" s="1">
+        <v>1</v>
+      </c>
+      <c r="N75" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="P75" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q75" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="K75" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="L75" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M75" s="1">
-        <v>1</v>
-      </c>
-      <c r="N75" s="1" t="s">
+      <c r="R75" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S75" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="U75" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="O75" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="P75" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q75" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="R75" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S75" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="U75" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="V75" s="2">
         <v>15.4017</v>
@@ -6904,10 +6895,10 @@
         <v>11</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>27</v>
@@ -6916,37 +6907,37 @@
         <v>4</v>
       </c>
       <c r="J76" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M76" s="1">
+        <v>1</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="O76" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="P76" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q76" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="K76" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="L76" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M76" s="1">
-        <v>1</v>
-      </c>
-      <c r="N76" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="O76" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="P76" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q76" s="1" t="s">
+      <c r="R76" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S76" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="U76" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="R76" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S76" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="U76" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="V76" s="2">
         <v>15.4018</v>
@@ -6972,10 +6963,10 @@
         <v>12</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>27</v>
@@ -6984,10 +6975,10 @@
         <v>16</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L77" s="1" t="s">
         <v>30</v>
@@ -6996,25 +6987,25 @@
         <v>8</v>
       </c>
       <c r="N77" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="O77" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="P77" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q77" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="R77" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S77" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U77" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="O77" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="P77" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q77" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="R77" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S77" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="U77" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="V77" s="2">
         <v>15.4018</v>
@@ -7040,10 +7031,10 @@
         <v>16</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>27</v>
@@ -7052,37 +7043,37 @@
         <v>17</v>
       </c>
       <c r="J78" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M78" s="1">
+        <v>23</v>
+      </c>
+      <c r="N78" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="O78" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="K78" s="1" t="s">
+      <c r="P78" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q78" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="L78" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M78" s="1">
-        <v>23</v>
-      </c>
-      <c r="N78" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="O78" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="P78" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q78" s="1" t="s">
-        <v>242</v>
-      </c>
       <c r="R78" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S78" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U78" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="V78" s="2">
         <v>15.4018</v>
@@ -7108,10 +7099,10 @@
         <v>18</v>
       </c>
       <c r="F79" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>27</v>
@@ -7120,37 +7111,37 @@
         <v>4</v>
       </c>
       <c r="J79" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K79" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="K79" s="1" t="s">
+      <c r="L79" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M79" s="1">
+        <v>1</v>
+      </c>
+      <c r="N79" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="L79" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M79" s="1">
-        <v>1</v>
-      </c>
-      <c r="N79" s="1" t="s">
+      <c r="O79" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="P79" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q79" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="O79" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="P79" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q79" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="R79" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S79" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U79" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="V79" s="2">
         <v>15.401899999999999</v>
@@ -7176,10 +7167,10 @@
         <v>18</v>
       </c>
       <c r="F80" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G80" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>27</v>
@@ -7188,37 +7179,37 @@
         <v>4</v>
       </c>
       <c r="J80" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K80" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="K80" s="1" t="s">
+      <c r="L80" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M80" s="1">
+        <v>1</v>
+      </c>
+      <c r="N80" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="L80" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M80" s="1">
-        <v>1</v>
-      </c>
-      <c r="N80" s="1" t="s">
+      <c r="O80" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="P80" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q80" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="O80" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="P80" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q80" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="R80" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S80" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U80" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="V80" s="2">
         <v>15.401899999999999</v>
@@ -7244,10 +7235,10 @@
         <v>18</v>
       </c>
       <c r="F81" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G81" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>27</v>
@@ -7256,37 +7247,37 @@
         <v>6</v>
       </c>
       <c r="J81" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K81" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K81" s="1" t="s">
+      <c r="L81" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M81" s="1">
+        <v>1</v>
+      </c>
+      <c r="N81" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L81" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M81" s="1">
-        <v>1</v>
-      </c>
-      <c r="N81" s="1" t="s">
+      <c r="O81" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="P81" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q81" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="O81" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="P81" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q81" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="R81" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S81" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="U81" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="V81" s="2">
         <v>15.401999999999999</v>
@@ -7312,10 +7303,10 @@
         <v>18</v>
       </c>
       <c r="F82" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G82" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>27</v>
@@ -7324,37 +7315,37 @@
         <v>6</v>
       </c>
       <c r="J82" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K82" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K82" s="1" t="s">
+      <c r="L82" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M82" s="1">
+        <v>1</v>
+      </c>
+      <c r="N82" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L82" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M82" s="1">
-        <v>1</v>
-      </c>
-      <c r="N82" s="1" t="s">
+      <c r="O82" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="P82" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q82" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="O82" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="P82" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q82" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="R82" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S82" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="U82" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="V82" s="2">
         <v>15.402100000000001</v>
@@ -7380,10 +7371,10 @@
         <v>18</v>
       </c>
       <c r="F83" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>27</v>
@@ -7392,37 +7383,37 @@
         <v>6</v>
       </c>
       <c r="J83" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K83" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K83" s="1" t="s">
+      <c r="L83" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M83" s="1">
+        <v>1</v>
+      </c>
+      <c r="N83" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L83" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M83" s="1">
-        <v>1</v>
-      </c>
-      <c r="N83" s="1" t="s">
+      <c r="O83" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="P83" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q83" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="O83" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="P83" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q83" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="R83" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S83" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="U83" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="U83" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="V83" s="2">
         <v>15.402100000000001</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-07-2020 05-14-25
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C33E569A-84F1-4469-A434-6BFB5A9DDECC}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{86AFD8AE-2489-454A-8701-DF969CBB1754}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="HOSPITALES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$93</definedName>
     <definedName name="_xlnm.Database">HOSPITALES!$A$1:$U$83</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="257">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -799,6 +799,12 @@
   </si>
   <si>
     <t>Hospital de Roatán</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mario Catarino Rivas </t>
+  </si>
+  <si>
+    <t>Leonardo Martínez</t>
   </si>
 </sst>
 </file>
@@ -1441,8 +1447,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W91" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W91" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W93" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W93" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W83">
     <sortCondition ref="S1:S83"/>
   </sortState>
@@ -1775,8 +1781,8 @@
   <dimension ref="A1:W91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="N75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R83" sqref="R83:R91"/>
+      <pane ySplit="1" topLeftCell="R81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V91" sqref="V91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -7453,12 +7459,27 @@
       </c>
     </row>
     <row r="84" spans="1:23">
+      <c r="B84" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D84" s="1">
+        <v>3</v>
+      </c>
       <c r="G84" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="H84" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K84" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="L84" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R84" s="1" t="s">
         <v>35</v>
       </c>
@@ -7479,12 +7500,27 @@
       </c>
     </row>
     <row r="85" spans="1:23">
+      <c r="B85" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D85" s="1">
+        <v>3</v>
+      </c>
       <c r="G85" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="H85" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K85" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="L85" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R85" s="1" t="s">
         <v>35</v>
       </c>
@@ -7505,12 +7541,27 @@
       </c>
     </row>
     <row r="86" spans="1:23">
+      <c r="B86" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D86" s="1">
+        <v>3</v>
+      </c>
       <c r="G86" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="H86" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K86" s="1" t="s">
         <v>252</v>
       </c>
+      <c r="L86" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R86" s="1" t="s">
         <v>35</v>
       </c>
@@ -7531,12 +7582,27 @@
       </c>
     </row>
     <row r="87" spans="1:23">
+      <c r="B87" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D87" s="1">
+        <v>3</v>
+      </c>
       <c r="G87" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="H87" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K87" s="1" t="s">
         <v>230</v>
       </c>
+      <c r="L87" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R87" s="1" t="s">
         <v>35</v>
       </c>
@@ -7557,6 +7623,27 @@
       </c>
     </row>
     <row r="88" spans="1:23">
+      <c r="B88" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D88" s="1">
+        <v>3</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L88" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R88" s="1" t="s">
         <v>35</v>
       </c>
@@ -7566,8 +7653,38 @@
       <c r="T88" s="1" t="s">
         <v>248</v>
       </c>
+      <c r="U88" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="V88" s="2">
+        <v>15.5245187</v>
+      </c>
+      <c r="W88" s="2">
+        <v>-88.043693599999997</v>
+      </c>
     </row>
     <row r="89" spans="1:23">
+      <c r="B89" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D89" s="1">
+        <v>3</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L89" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R89" s="1" t="s">
         <v>35</v>
       </c>
@@ -7577,8 +7694,32 @@
       <c r="T89" s="1" t="s">
         <v>248</v>
       </c>
+      <c r="U89" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="V89" s="2">
+        <v>15.500535899999999</v>
+      </c>
+      <c r="W89" s="2">
+        <v>-88.0310652</v>
+      </c>
     </row>
     <row r="90" spans="1:23">
+      <c r="B90" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D90" s="1">
+        <v>3</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L90" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R90" s="1" t="s">
         <v>35</v>
       </c>
@@ -7588,8 +7729,29 @@
       <c r="T90" s="1" t="s">
         <v>248</v>
       </c>
+      <c r="V90" s="2">
+        <v>13.3077843</v>
+      </c>
+      <c r="W90" s="2">
+        <v>-87.207522900000001</v>
+      </c>
     </row>
     <row r="91" spans="1:23">
+      <c r="B91" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D91" s="1">
+        <v>3</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L91" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R91" s="1" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-07-2020 17-43-31
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -1781,8 +1781,8 @@
   <dimension ref="A1:W91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="R81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V91" sqref="V91"/>
+      <pane ySplit="1" topLeftCell="P81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W84" sqref="W84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-07-2020 19-09-21
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{86AFD8AE-2489-454A-8701-DF969CBB1754}"/>
+  <xr:revisionPtr revIDLastSave="204" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9C432C62-00D2-49AC-B510-6A8330D12FE6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="259">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -801,10 +801,16 @@
     <t>Hospital de Roatán</t>
   </si>
   <si>
-    <t xml:space="preserve">Mario Catarino Rivas </t>
-  </si>
-  <si>
-    <t>Leonardo Martínez</t>
+    <t xml:space="preserve">Hospital Nacional Nor-Occidental Mario Catarino Rivas </t>
+  </si>
+  <si>
+    <t>Hospital Leonardo Martínez Valenzuela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puerto Cortés </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital Puerto Cortés </t>
   </si>
 </sst>
 </file>
@@ -1781,8 +1787,8 @@
   <dimension ref="A1:W91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="P81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W84" sqref="W84"/>
+      <pane ySplit="1" topLeftCell="C80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G99" sqref="G98:G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -7493,10 +7499,10 @@
         <v>249</v>
       </c>
       <c r="V84" s="2">
-        <v>14.105252200000001</v>
+        <v>14.104480000000001</v>
       </c>
       <c r="W84" s="2">
-        <v>-87.184888599999994</v>
+        <v>-87.182319000000007</v>
       </c>
     </row>
     <row r="85" spans="1:23">
@@ -7534,10 +7540,10 @@
         <v>250</v>
       </c>
       <c r="V85" s="2">
-        <v>14.103733999999999</v>
+        <v>14.103702999999999</v>
       </c>
       <c r="W85" s="2">
-        <v>-87.186564300000001</v>
+        <v>-87.185029999999998</v>
       </c>
     </row>
     <row r="86" spans="1:23">
@@ -7575,10 +7581,10 @@
         <v>253</v>
       </c>
       <c r="V86" s="2">
-        <v>13.991437899999999</v>
+        <v>13.991413</v>
       </c>
       <c r="W86" s="2">
-        <v>-86.5703362</v>
+        <v>-86.568146999999996</v>
       </c>
     </row>
     <row r="87" spans="1:23">
@@ -7616,10 +7622,10 @@
         <v>254</v>
       </c>
       <c r="V87" s="2">
-        <v>16.358969900000002</v>
+        <v>16.317903000000001</v>
       </c>
       <c r="W87" s="2">
-        <v>-86.5382848</v>
+        <v>-86.539259000000001</v>
       </c>
     </row>
     <row r="88" spans="1:23">
@@ -7657,10 +7663,10 @@
         <v>255</v>
       </c>
       <c r="V88" s="2">
-        <v>15.5245187</v>
+        <v>15.524452999999999</v>
       </c>
       <c r="W88" s="2">
-        <v>-88.043693599999997</v>
+        <v>-88.041515000000004</v>
       </c>
     </row>
     <row r="89" spans="1:23">
@@ -7698,10 +7704,10 @@
         <v>256</v>
       </c>
       <c r="V89" s="2">
-        <v>15.500535899999999</v>
+        <v>15.500176</v>
       </c>
       <c r="W89" s="2">
-        <v>-88.0310652</v>
+        <v>-88.030754999999999</v>
       </c>
     </row>
     <row r="90" spans="1:23">
@@ -7714,8 +7720,14 @@
       <c r="D90" s="1">
         <v>3</v>
       </c>
+      <c r="G90" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="H90" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>257</v>
       </c>
       <c r="L90" s="1" t="s">
         <v>30</v>
@@ -7729,11 +7741,14 @@
       <c r="T90" s="1" t="s">
         <v>248</v>
       </c>
+      <c r="U90" s="1" t="s">
+        <v>258</v>
+      </c>
       <c r="V90" s="2">
-        <v>13.3077843</v>
+        <v>15.814730000000001</v>
       </c>
       <c r="W90" s="2">
-        <v>-87.207522900000001</v>
+        <v>-87.936245</v>
       </c>
     </row>
     <row r="91" spans="1:23">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-07-2020 20-35-13
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9C432C62-00D2-49AC-B510-6A8330D12FE6}"/>
+  <xr:revisionPtr revIDLastSave="282" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{521ABC66-966A-4C87-B8EC-72C98C115409}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="HOSPITALES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$96</definedName>
     <definedName name="_xlnm.Database">HOSPITALES!$A$1:$U$83</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="271">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -171,405 +171,405 @@
     <t>Centro de Salud</t>
   </si>
   <si>
+    <t>0105</t>
+  </si>
+  <si>
+    <t>La Masica</t>
+  </si>
+  <si>
+    <t>010514</t>
+  </si>
+  <si>
+    <t>San Juan Pueblo</t>
+  </si>
+  <si>
+    <t>HND-0105</t>
+  </si>
+  <si>
+    <t>Centro de Salud Isolina Ruíz</t>
+  </si>
+  <si>
+    <t>Centro de Salud El Manchen</t>
+  </si>
+  <si>
+    <t>Centro Salud Sagrada Familia</t>
+  </si>
+  <si>
+    <t>Centro de Salud El Chile</t>
+  </si>
+  <si>
+    <t>Centro de Salud El Bosque</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Islas de La Bahía</t>
+  </si>
+  <si>
+    <t>1104</t>
+  </si>
+  <si>
+    <t>Útila</t>
+  </si>
+  <si>
+    <t>110401</t>
+  </si>
+  <si>
+    <t>HND-1104</t>
+  </si>
+  <si>
+    <t>Centro De Salud - Clinic</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>La Paz</t>
+  </si>
+  <si>
+    <t>1216</t>
+  </si>
+  <si>
+    <t>Santa Elena</t>
+  </si>
+  <si>
+    <t>121608</t>
+  </si>
+  <si>
+    <t>Nahuaterique</t>
+  </si>
+  <si>
+    <t>HND-1216</t>
+  </si>
+  <si>
+    <t>Centro de salud Nahuaterique</t>
+  </si>
+  <si>
+    <t>010103</t>
+  </si>
+  <si>
+    <t>Bonitillo</t>
+  </si>
+  <si>
+    <t>clínica</t>
+  </si>
+  <si>
+    <t>Clínica Metodista</t>
+  </si>
+  <si>
+    <t>Clínica De Especialdades</t>
+  </si>
+  <si>
+    <t>Emergencias Médicas</t>
+  </si>
+  <si>
+    <t>Clínica Médica Edgar Padilla</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>Copán</t>
+  </si>
+  <si>
+    <t>0402</t>
+  </si>
+  <si>
+    <t>Cabañas</t>
+  </si>
+  <si>
+    <t>040201</t>
+  </si>
+  <si>
+    <t>HND-0402</t>
+  </si>
+  <si>
+    <t>M.Y.V</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>Cortés</t>
+  </si>
+  <si>
+    <t>0501</t>
+  </si>
+  <si>
+    <t>San Pedro Sula</t>
+  </si>
+  <si>
+    <t>050101</t>
+  </si>
+  <si>
+    <t>HND-0501</t>
+  </si>
+  <si>
+    <t>Clínica Ferraro</t>
+  </si>
+  <si>
+    <t>Clínica Dentales Unidas</t>
+  </si>
+  <si>
+    <t>0506</t>
+  </si>
+  <si>
+    <t>Puerto Cortés</t>
+  </si>
+  <si>
+    <t>050601</t>
+  </si>
+  <si>
+    <t>HND-0506</t>
+  </si>
+  <si>
+    <t>Cruz Roja Hondureña</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Choluteca</t>
+  </si>
+  <si>
+    <t>0601</t>
+  </si>
+  <si>
+    <t>060101</t>
+  </si>
+  <si>
+    <t>HND-0601</t>
+  </si>
+  <si>
+    <t>Clínica San Francisco de Asís</t>
+  </si>
+  <si>
+    <t>Ashonplafa</t>
+  </si>
+  <si>
+    <t>Clínica Santa María</t>
+  </si>
+  <si>
+    <t>0606</t>
+  </si>
+  <si>
+    <t>El Triunfo</t>
+  </si>
+  <si>
+    <t>060603</t>
+  </si>
+  <si>
+    <t>El Cedrito</t>
+  </si>
+  <si>
+    <t>HND-0606</t>
+  </si>
+  <si>
+    <t>Clínica Médica Gosén</t>
+  </si>
+  <si>
+    <t>Laboratorio y Droguería Francelia</t>
+  </si>
+  <si>
+    <t>Clínica Clíper Hato de Enmedio</t>
+  </si>
+  <si>
+    <t>Asociación Pediatrica Hondureña</t>
+  </si>
+  <si>
+    <t>Centro Integral de Atención al Diabetico - CIAD</t>
+  </si>
+  <si>
+    <t>Clínicas Médicas</t>
+  </si>
+  <si>
+    <t>Dental Line</t>
+  </si>
+  <si>
+    <t>Óptica Robles</t>
+  </si>
+  <si>
+    <t>Laboratorio Palmira</t>
+  </si>
+  <si>
+    <t>Prolab</t>
+  </si>
+  <si>
+    <t>Clínica Rivera</t>
+  </si>
+  <si>
+    <t>Hospital y Clínicas Viera</t>
+  </si>
+  <si>
+    <t>Clínica Salesiano</t>
+  </si>
+  <si>
+    <t>080111</t>
+  </si>
+  <si>
+    <t>El Piliguan</t>
+  </si>
+  <si>
+    <t>CLIPER</t>
+  </si>
+  <si>
+    <t>0806</t>
+  </si>
+  <si>
+    <t>Guaimaca</t>
+  </si>
+  <si>
+    <t>080601</t>
+  </si>
+  <si>
+    <t>HND-0806</t>
+  </si>
+  <si>
+    <t>Clínica ENGA-DI</t>
+  </si>
+  <si>
+    <t>Clínica Criolla</t>
+  </si>
+  <si>
+    <t>Clínica de Emergencias Médicas</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Intibucá</t>
+  </si>
+  <si>
+    <t>1007</t>
+  </si>
+  <si>
+    <t>Jesús de Otoro</t>
+  </si>
+  <si>
+    <t>100701</t>
+  </si>
+  <si>
+    <t>HND-1007</t>
+  </si>
+  <si>
+    <t>Centro de Salud Camilo Giron Rivera</t>
+  </si>
+  <si>
+    <t>Clínica Santa Fe</t>
+  </si>
+  <si>
+    <t>Materno Infantil</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Lempira</t>
+  </si>
+  <si>
+    <t>1301</t>
+  </si>
+  <si>
+    <t>Gracias</t>
+  </si>
+  <si>
+    <t>130101</t>
+  </si>
+  <si>
+    <t>HND-1301</t>
+  </si>
+  <si>
+    <t>San Lucas</t>
+  </si>
+  <si>
+    <t>1311</t>
+  </si>
+  <si>
+    <t>La Unión</t>
+  </si>
+  <si>
+    <t>131101</t>
+  </si>
+  <si>
+    <t>HND-1311</t>
+  </si>
+  <si>
+    <t>Clínica Médica Vida Abundante</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Olancho</t>
+  </si>
+  <si>
+    <t>1505</t>
+  </si>
+  <si>
+    <t>Dulce Nombre de Culmí</t>
+  </si>
+  <si>
+    <t>150501</t>
+  </si>
+  <si>
+    <t>HND-1505</t>
+  </si>
+  <si>
+    <t>Clínica Sinaí</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Yoro</t>
+  </si>
+  <si>
+    <t>1804</t>
+  </si>
+  <si>
+    <t>El Progreso</t>
+  </si>
+  <si>
+    <t>180401</t>
+  </si>
+  <si>
+    <t>HND-1804</t>
+  </si>
+  <si>
+    <t>Clínica del Ojo</t>
+  </si>
+  <si>
+    <t>1806</t>
+  </si>
+  <si>
+    <t>Morazán</t>
+  </si>
+  <si>
+    <t>180601</t>
+  </si>
+  <si>
+    <t>HND-1806</t>
+  </si>
+  <si>
+    <t>Policlínica San Jorge</t>
+  </si>
+  <si>
+    <t>farmacia</t>
+  </si>
+  <si>
+    <t>Farmacia Simán</t>
+  </si>
+  <si>
+    <t>Farmacia Kielsa</t>
+  </si>
+  <si>
+    <t>Farmacia Bethania</t>
+  </si>
+  <si>
     <t>Atlantida</t>
   </si>
   <si>
-    <t>0105</t>
-  </si>
-  <si>
-    <t>La Masica</t>
-  </si>
-  <si>
-    <t>010514</t>
-  </si>
-  <si>
-    <t>San Juan Pueblo</t>
-  </si>
-  <si>
-    <t>HND-0105</t>
-  </si>
-  <si>
-    <t>Centro de Salud Isolina Ruíz</t>
-  </si>
-  <si>
-    <t>Centro de Salud El Manchen</t>
-  </si>
-  <si>
-    <t>Centro Salud Sagrada Familia</t>
-  </si>
-  <si>
-    <t>Centro de Salud El Chile</t>
-  </si>
-  <si>
-    <t>Centro de Salud El Bosque</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Islas de La Bahía</t>
-  </si>
-  <si>
-    <t>1104</t>
-  </si>
-  <si>
-    <t>Útila</t>
-  </si>
-  <si>
-    <t>110401</t>
-  </si>
-  <si>
-    <t>HND-1104</t>
-  </si>
-  <si>
-    <t>Centro De Salud - Clinic</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>La Paz</t>
-  </si>
-  <si>
-    <t>1216</t>
-  </si>
-  <si>
-    <t>Santa Elena</t>
-  </si>
-  <si>
-    <t>121608</t>
-  </si>
-  <si>
-    <t>Nahuaterique</t>
-  </si>
-  <si>
-    <t>HND-1216</t>
-  </si>
-  <si>
-    <t>Centro de salud Nahuaterique</t>
-  </si>
-  <si>
-    <t>010103</t>
-  </si>
-  <si>
-    <t>Bonitillo</t>
-  </si>
-  <si>
-    <t>clínica</t>
-  </si>
-  <si>
-    <t>Clínica Metodista</t>
-  </si>
-  <si>
-    <t>Clínica De Especialdades</t>
-  </si>
-  <si>
-    <t>Emergencias Médicas</t>
-  </si>
-  <si>
-    <t>Clínica Médica Edgar Padilla</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>Copán</t>
-  </si>
-  <si>
-    <t>0402</t>
-  </si>
-  <si>
-    <t>Cabañas</t>
-  </si>
-  <si>
-    <t>040201</t>
-  </si>
-  <si>
-    <t>HND-0402</t>
-  </si>
-  <si>
-    <t>M.Y.V</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>Cortés</t>
-  </si>
-  <si>
-    <t>0501</t>
-  </si>
-  <si>
-    <t>San Pedro Sula</t>
-  </si>
-  <si>
-    <t>050101</t>
-  </si>
-  <si>
-    <t>HND-0501</t>
-  </si>
-  <si>
-    <t>Clínica Ferraro</t>
-  </si>
-  <si>
-    <t>Clínica Dentales Unidas</t>
-  </si>
-  <si>
-    <t>0506</t>
-  </si>
-  <si>
-    <t>Puerto Cortés</t>
-  </si>
-  <si>
-    <t>050601</t>
-  </si>
-  <si>
-    <t>HND-0506</t>
-  </si>
-  <si>
-    <t>Cruz Roja Hondureña</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>Choluteca</t>
-  </si>
-  <si>
-    <t>0601</t>
-  </si>
-  <si>
-    <t>060101</t>
-  </si>
-  <si>
-    <t>HND-0601</t>
-  </si>
-  <si>
-    <t>Clínica San Francisco de Asís</t>
-  </si>
-  <si>
-    <t>Ashonplafa</t>
-  </si>
-  <si>
-    <t>Clínica Santa María</t>
-  </si>
-  <si>
-    <t>0606</t>
-  </si>
-  <si>
-    <t>El Triunfo</t>
-  </si>
-  <si>
-    <t>060603</t>
-  </si>
-  <si>
-    <t>El Cedrito</t>
-  </si>
-  <si>
-    <t>HND-0606</t>
-  </si>
-  <si>
-    <t>Clínica Médica Gosén</t>
-  </si>
-  <si>
-    <t>Laboratorio y Droguería Francelia</t>
-  </si>
-  <si>
-    <t>Clínica Clíper Hato de Enmedio</t>
-  </si>
-  <si>
-    <t>Asociación Pediatrica Hondureña</t>
-  </si>
-  <si>
-    <t>Centro Integral de Atención al Diabetico - CIAD</t>
-  </si>
-  <si>
-    <t>Clínicas Médicas</t>
-  </si>
-  <si>
-    <t>Dental Line</t>
-  </si>
-  <si>
-    <t>Óptica Robles</t>
-  </si>
-  <si>
-    <t>Laboratorio Palmira</t>
-  </si>
-  <si>
-    <t>Prolab</t>
-  </si>
-  <si>
-    <t>Clínica Rivera</t>
-  </si>
-  <si>
-    <t>Hospital y Clínicas Viera</t>
-  </si>
-  <si>
-    <t>Clínica Salesiano</t>
-  </si>
-  <si>
-    <t>080111</t>
-  </si>
-  <si>
-    <t>El Piliguan</t>
-  </si>
-  <si>
-    <t>CLIPER</t>
-  </si>
-  <si>
-    <t>0806</t>
-  </si>
-  <si>
-    <t>Guaimaca</t>
-  </si>
-  <si>
-    <t>080601</t>
-  </si>
-  <si>
-    <t>HND-0806</t>
-  </si>
-  <si>
-    <t>Clínica ENGA-DI</t>
-  </si>
-  <si>
-    <t>Clínica Criolla</t>
-  </si>
-  <si>
-    <t>Clínica de Emergencias Médicas</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Intibucá</t>
-  </si>
-  <si>
-    <t>1007</t>
-  </si>
-  <si>
-    <t>Jesús de Otoro</t>
-  </si>
-  <si>
-    <t>100701</t>
-  </si>
-  <si>
-    <t>HND-1007</t>
-  </si>
-  <si>
-    <t>Centro de Salud Camilo Giron Rivera</t>
-  </si>
-  <si>
-    <t>Clínica Santa Fe</t>
-  </si>
-  <si>
-    <t>Materno Infantil</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Lempira</t>
-  </si>
-  <si>
-    <t>1301</t>
-  </si>
-  <si>
-    <t>Gracias</t>
-  </si>
-  <si>
-    <t>130101</t>
-  </si>
-  <si>
-    <t>HND-1301</t>
-  </si>
-  <si>
-    <t>San Lucas</t>
-  </si>
-  <si>
-    <t>1311</t>
-  </si>
-  <si>
-    <t>La Unión</t>
-  </si>
-  <si>
-    <t>131101</t>
-  </si>
-  <si>
-    <t>HND-1311</t>
-  </si>
-  <si>
-    <t>Clínica Médica Vida Abundante</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Olancho</t>
-  </si>
-  <si>
-    <t>1505</t>
-  </si>
-  <si>
-    <t>Dulce Nombre de Culmí</t>
-  </si>
-  <si>
-    <t>150501</t>
-  </si>
-  <si>
-    <t>HND-1505</t>
-  </si>
-  <si>
-    <t>Clínica Sinaí</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Yoro</t>
-  </si>
-  <si>
-    <t>1804</t>
-  </si>
-  <si>
-    <t>El Progreso</t>
-  </si>
-  <si>
-    <t>180401</t>
-  </si>
-  <si>
-    <t>HND-1804</t>
-  </si>
-  <si>
-    <t>Clínica del Ojo</t>
-  </si>
-  <si>
-    <t>1806</t>
-  </si>
-  <si>
-    <t>Morazán</t>
-  </si>
-  <si>
-    <t>180601</t>
-  </si>
-  <si>
-    <t>HND-1806</t>
-  </si>
-  <si>
-    <t>Policlínica San Jorge</t>
-  </si>
-  <si>
-    <t>farmacia</t>
-  </si>
-  <si>
-    <t>Farmacia Simán</t>
-  </si>
-  <si>
-    <t>Farmacia Kielsa</t>
-  </si>
-  <si>
-    <t>Farmacia Bethania</t>
-  </si>
-  <si>
     <t>010101</t>
   </si>
   <si>
@@ -811,6 +811,42 @@
   </si>
   <si>
     <t xml:space="preserve">Hospital Puerto Cortés </t>
+  </si>
+  <si>
+    <t>Hospital Regional del Sur</t>
+  </si>
+  <si>
+    <t>Hospital Atlántida</t>
+  </si>
+  <si>
+    <t>Santa Rosa de Copán</t>
+  </si>
+  <si>
+    <t>Hospital de Occidente</t>
+  </si>
+  <si>
+    <t>Trujillo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital Salvador Paredes </t>
+  </si>
+  <si>
+    <t>Ocotepeque</t>
+  </si>
+  <si>
+    <t>San Marcos</t>
+  </si>
+  <si>
+    <t>Hospital San Marcos de Ocotepeque</t>
+  </si>
+  <si>
+    <t>Valle</t>
+  </si>
+  <si>
+    <t>San Lorenzo</t>
+  </si>
+  <si>
+    <t>Hospital San Lorenzo</t>
   </si>
 </sst>
 </file>
@@ -1453,8 +1489,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W93" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W93" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W96" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W96" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W83">
     <sortCondition ref="S1:S83"/>
   </sortState>
@@ -1784,11 +1820,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W91"/>
+  <dimension ref="A1:W96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="C80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G99" sqref="G98:G99"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -2044,7 +2080,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>27</v>
@@ -2053,10 +2089,10 @@
         <v>5</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>30</v>
@@ -2065,16 +2101,16 @@
         <v>14</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>35</v>
@@ -2083,7 +2119,7 @@
         <v>36</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V4" s="2">
         <v>15.399800000000001</v>
@@ -2151,7 +2187,7 @@
         <v>36</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V5" s="2">
         <v>15.401400000000001</v>
@@ -2219,7 +2255,7 @@
         <v>36</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V6" s="2">
         <v>15.401400000000001</v>
@@ -2287,7 +2323,7 @@
         <v>36</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V7" s="2">
         <v>15.4016</v>
@@ -2355,7 +2391,7 @@
         <v>36</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V8" s="2">
         <v>15.4016</v>
@@ -2381,10 +2417,10 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>27</v>
@@ -2393,28 +2429,28 @@
         <v>4</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M9" s="1">
-        <v>1</v>
-      </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>35</v>
@@ -2423,7 +2459,7 @@
         <v>36</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V9" s="2">
         <v>15.4016</v>
@@ -2449,10 +2485,10 @@
         <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>27</v>
@@ -2461,10 +2497,10 @@
         <v>16</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>30</v>
@@ -2473,16 +2509,16 @@
         <v>8</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>35</v>
@@ -2491,7 +2527,7 @@
         <v>36</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V10" s="2">
         <v>15.4018</v>
@@ -2541,10 +2577,10 @@
         <v>3</v>
       </c>
       <c r="N11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>33</v>
@@ -2556,10 +2592,10 @@
         <v>35</v>
       </c>
       <c r="S11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U11" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="V11" s="2">
         <v>14.157299999999999</v>
@@ -2597,10 +2633,10 @@
         <v>5</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>30</v>
@@ -2609,25 +2645,25 @@
         <v>14</v>
       </c>
       <c r="N12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="R12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="V12" s="2">
         <v>14.068899999999999</v>
@@ -2665,10 +2701,10 @@
         <v>5</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>30</v>
@@ -2677,25 +2713,25 @@
         <v>14</v>
       </c>
       <c r="N13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="R13" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V13" s="2">
         <v>14.0501</v>
@@ -2733,10 +2769,10 @@
         <v>5</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>30</v>
@@ -2745,25 +2781,25 @@
         <v>14</v>
       </c>
       <c r="N14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="R14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V14" s="2">
         <v>14.3118</v>
@@ -2789,10 +2825,10 @@
         <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>27</v>
@@ -2801,37 +2837,37 @@
         <v>2</v>
       </c>
       <c r="J15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M15" s="1">
-        <v>1</v>
-      </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q15" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q15" s="1" t="s">
+      <c r="R15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U15" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="V15" s="2">
         <v>14.3165</v>
@@ -2857,46 +2893,46 @@
         <v>5</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="1">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M16" s="1">
-        <v>1</v>
-      </c>
-      <c r="N16" s="1" t="s">
+      <c r="O16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q16" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O16" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="R16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>44</v>
@@ -2925,46 +2961,46 @@
         <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" s="1">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M17" s="1">
-        <v>1</v>
-      </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q17" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O17" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="R17" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>44</v>
@@ -2993,46 +3029,46 @@
         <v>5</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I18" s="1">
-        <v>1</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1</v>
+      </c>
+      <c r="N18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M18" s="1">
-        <v>1</v>
-      </c>
-      <c r="N18" s="1" t="s">
+      <c r="O18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q18" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="R18" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>44</v>
@@ -3061,49 +3097,49 @@
         <v>5</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" s="1">
-        <v>1</v>
-      </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M19" s="1">
-        <v>1</v>
-      </c>
-      <c r="N19" s="1" t="s">
+      <c r="O19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q19" s="1" t="s">
+      <c r="R19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U19" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="V19" s="2">
         <v>14.245100000000001</v>
@@ -3129,49 +3165,49 @@
         <v>5</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="1">
-        <v>1</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M20" s="1">
-        <v>1</v>
-      </c>
-      <c r="N20" s="1" t="s">
+      <c r="O20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q20" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="R20" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V20" s="2">
         <v>14.246</v>
@@ -3197,10 +3233,10 @@
         <v>5</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>27</v>
@@ -3209,37 +3245,37 @@
         <v>6</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21" s="1">
+        <v>1</v>
+      </c>
+      <c r="N21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M21" s="1">
-        <v>1</v>
-      </c>
-      <c r="N21" s="1" t="s">
+      <c r="O21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q21" s="1" t="s">
+      <c r="R21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U21" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="V21" s="2">
         <v>14.579700000000001</v>
@@ -3265,49 +3301,49 @@
         <v>6</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22" s="1">
-        <v>1</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M22" s="1">
-        <v>1</v>
-      </c>
-      <c r="N22" s="1" t="s">
+      <c r="O22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q22" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O22" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q22" s="1" t="s">
+      <c r="R22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U22" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="V22" s="2">
         <v>14.5837</v>
@@ -3333,49 +3369,49 @@
         <v>6</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I23" s="1">
-        <v>1</v>
-      </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1</v>
+      </c>
+      <c r="N23" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M23" s="1">
-        <v>1</v>
-      </c>
-      <c r="N23" s="1" t="s">
+      <c r="O23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q23" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="R23" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="V23" s="2">
         <v>14.5839</v>
@@ -3401,49 +3437,49 @@
         <v>6</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24" s="1">
-        <v>1</v>
-      </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M24" s="1">
+        <v>1</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M24" s="1">
-        <v>1</v>
-      </c>
-      <c r="N24" s="1" t="s">
+      <c r="O24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O24" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="R24" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V24" s="2">
         <v>14.5844</v>
@@ -3469,10 +3505,10 @@
         <v>6</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>27</v>
@@ -3481,37 +3517,37 @@
         <v>6</v>
       </c>
       <c r="J25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M25" s="1">
+        <v>3</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M25" s="1">
-        <v>3</v>
-      </c>
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q25" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="P25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q25" s="1" t="s">
+      <c r="R25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U25" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U25" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="V25" s="2">
         <v>14.5852</v>
@@ -3576,10 +3612,10 @@
         <v>35</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V26" s="2">
         <v>14.5854</v>
@@ -3644,10 +3680,10 @@
         <v>35</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V27" s="2">
         <v>14.5855</v>
@@ -3712,10 +3748,10 @@
         <v>35</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V28" s="2">
         <v>14.585699999999999</v>
@@ -3780,10 +3816,10 @@
         <v>35</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="V29" s="2">
         <v>14.585699999999999</v>
@@ -3848,10 +3884,10 @@
         <v>35</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V30" s="2">
         <v>14.585900000000001</v>
@@ -3916,10 +3952,10 @@
         <v>35</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V31" s="2">
         <v>14.585900000000001</v>
@@ -3984,10 +4020,10 @@
         <v>35</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U32" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="V32" s="2">
         <v>14.5862</v>
@@ -4052,10 +4088,10 @@
         <v>35</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U33" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="V33" s="2">
         <v>14.5869</v>
@@ -4120,10 +4156,10 @@
         <v>35</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="V34" s="2">
         <v>14.587300000000001</v>
@@ -4188,10 +4224,10 @@
         <v>35</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V35" s="2">
         <v>14.5875</v>
@@ -4256,10 +4292,10 @@
         <v>35</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V36" s="2">
         <v>14.5877</v>
@@ -4324,10 +4360,10 @@
         <v>35</v>
       </c>
       <c r="S37" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V37" s="2">
         <v>14.5878</v>
@@ -4392,10 +4428,10 @@
         <v>35</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V38" s="2">
         <v>14.587899999999999</v>
@@ -4445,10 +4481,10 @@
         <v>11</v>
       </c>
       <c r="N39" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O39" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="P39" s="1" t="s">
         <v>33</v>
@@ -4460,10 +4496,10 @@
         <v>35</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="V39" s="2">
         <v>14.587999999999999</v>
@@ -4501,37 +4537,37 @@
         <v>6</v>
       </c>
       <c r="J40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K40" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M40" s="1">
+        <v>1</v>
+      </c>
+      <c r="N40" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M40" s="1">
-        <v>1</v>
-      </c>
-      <c r="N40" s="1" t="s">
+      <c r="O40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q40" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="O40" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q40" s="1" t="s">
+      <c r="R40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U40" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="R40" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S40" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U40" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="V40" s="2">
         <v>14.588200000000001</v>
@@ -4569,37 +4605,37 @@
         <v>6</v>
       </c>
       <c r="J41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K41" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M41" s="1">
+        <v>1</v>
+      </c>
+      <c r="N41" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M41" s="1">
-        <v>1</v>
-      </c>
-      <c r="N41" s="1" t="s">
+      <c r="O41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q41" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="O41" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="R41" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U41" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="V41" s="2">
         <v>14.588200000000001</v>
@@ -4637,37 +4673,37 @@
         <v>6</v>
       </c>
       <c r="J42" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K42" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="L42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M42" s="1">
+        <v>1</v>
+      </c>
+      <c r="N42" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="L42" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M42" s="1">
-        <v>1</v>
-      </c>
-      <c r="N42" s="1" t="s">
+      <c r="O42" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q42" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="O42" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="R42" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S42" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U42" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V42" s="2">
         <v>14.5883</v>
@@ -4693,10 +4729,10 @@
         <v>10</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>27</v>
@@ -4705,37 +4741,37 @@
         <v>7</v>
       </c>
       <c r="J43" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K43" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="L43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M43" s="1">
+        <v>1</v>
+      </c>
+      <c r="N43" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L43" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M43" s="1">
-        <v>1</v>
-      </c>
-      <c r="N43" s="1" t="s">
+      <c r="O43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q43" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="O43" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="R43" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S43" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U43" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="V43" s="2">
         <v>14.5885</v>
@@ -4761,10 +4797,10 @@
         <v>10</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>27</v>
@@ -4773,37 +4809,37 @@
         <v>7</v>
       </c>
       <c r="J44" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K44" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="L44" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M44" s="1">
+        <v>1</v>
+      </c>
+      <c r="N44" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M44" s="1">
-        <v>1</v>
-      </c>
-      <c r="N44" s="1" t="s">
+      <c r="O44" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q44" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="O44" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q44" s="1" t="s">
+      <c r="R44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U44" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="R44" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S44" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U44" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="V44" s="2">
         <v>14.5886</v>
@@ -4829,10 +4865,10 @@
         <v>10</v>
       </c>
       <c r="F45" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>27</v>
@@ -4841,37 +4877,37 @@
         <v>7</v>
       </c>
       <c r="J45" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="L45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M45" s="1">
+        <v>1</v>
+      </c>
+      <c r="N45" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L45" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M45" s="1">
-        <v>1</v>
-      </c>
-      <c r="N45" s="1" t="s">
+      <c r="O45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q45" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="O45" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="P45" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q45" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="R45" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U45" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="V45" s="2">
         <v>14.5886</v>
@@ -4897,10 +4933,10 @@
         <v>10</v>
       </c>
       <c r="F46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>27</v>
@@ -4909,37 +4945,37 @@
         <v>7</v>
       </c>
       <c r="J46" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K46" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="L46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M46" s="1">
+        <v>1</v>
+      </c>
+      <c r="N46" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L46" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M46" s="1">
-        <v>1</v>
-      </c>
-      <c r="N46" s="1" t="s">
+      <c r="O46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q46" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="O46" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="P46" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q46" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="R46" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U46" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V46" s="2">
         <v>14.588699999999999</v>
@@ -4965,49 +5001,49 @@
         <v>13</v>
       </c>
       <c r="F47" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="H47" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I47" s="1">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I47" s="1">
-        <v>1</v>
-      </c>
-      <c r="J47" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="L47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M47" s="1">
+        <v>1</v>
+      </c>
+      <c r="N47" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="L47" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M47" s="1">
-        <v>1</v>
-      </c>
-      <c r="N47" s="1" t="s">
+      <c r="O47" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q47" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="O47" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="P47" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q47" s="1" t="s">
+      <c r="R47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S47" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U47" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="R47" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S47" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U47" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="V47" s="2">
         <v>14.588699999999999</v>
@@ -5033,10 +5069,10 @@
         <v>13</v>
       </c>
       <c r="F48" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>27</v>
@@ -5045,37 +5081,37 @@
         <v>11</v>
       </c>
       <c r="J48" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K48" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="L48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M48" s="1">
+        <v>1</v>
+      </c>
+      <c r="N48" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="L48" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M48" s="1">
-        <v>1</v>
-      </c>
-      <c r="N48" s="1" t="s">
+      <c r="O48" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q48" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="O48" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q48" s="1" t="s">
+      <c r="R48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S48" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U48" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="R48" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S48" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U48" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="V48" s="2">
         <v>14.588800000000001</v>
@@ -5101,10 +5137,10 @@
         <v>15</v>
       </c>
       <c r="F49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>27</v>
@@ -5113,37 +5149,37 @@
         <v>5</v>
       </c>
       <c r="J49" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K49" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="L49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M49" s="1">
+        <v>1</v>
+      </c>
+      <c r="N49" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="L49" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M49" s="1">
-        <v>1</v>
-      </c>
-      <c r="N49" s="1" t="s">
+      <c r="O49" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q49" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="O49" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="P49" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q49" s="1" t="s">
+      <c r="R49" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S49" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U49" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="R49" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S49" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U49" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="V49" s="2">
         <v>14.588800000000001</v>
@@ -5169,10 +5205,10 @@
         <v>18</v>
       </c>
       <c r="F50" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>27</v>
@@ -5181,37 +5217,37 @@
         <v>4</v>
       </c>
       <c r="J50" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K50" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="L50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M50" s="1">
+        <v>1</v>
+      </c>
+      <c r="N50" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="L50" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M50" s="1">
-        <v>1</v>
-      </c>
-      <c r="N50" s="1" t="s">
+      <c r="O50" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q50" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="O50" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="P50" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q50" s="1" t="s">
+      <c r="R50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S50" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U50" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="R50" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S50" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U50" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="V50" s="2">
         <v>14.588900000000001</v>
@@ -5237,10 +5273,10 @@
         <v>18</v>
       </c>
       <c r="F51" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>27</v>
@@ -5249,37 +5285,37 @@
         <v>6</v>
       </c>
       <c r="J51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K51" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="L51" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M51" s="1">
+        <v>1</v>
+      </c>
+      <c r="N51" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="L51" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M51" s="1">
-        <v>1</v>
-      </c>
-      <c r="N51" s="1" t="s">
+      <c r="O51" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q51" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="O51" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="P51" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q51" s="1" t="s">
+      <c r="R51" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U51" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="R51" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S51" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U51" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="V51" s="2">
         <v>14.588900000000001</v>
@@ -5305,10 +5341,10 @@
         <v>18</v>
       </c>
       <c r="F52" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>27</v>
@@ -5317,37 +5353,37 @@
         <v>6</v>
       </c>
       <c r="J52" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K52" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K52" s="1" t="s">
+      <c r="L52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M52" s="1">
+        <v>1</v>
+      </c>
+      <c r="N52" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="L52" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M52" s="1">
-        <v>1</v>
-      </c>
-      <c r="N52" s="1" t="s">
+      <c r="O52" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q52" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="O52" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q52" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="R52" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S52" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="U52" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="U52" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="V52" s="2">
         <v>15.401999999999999</v>
@@ -5373,10 +5409,10 @@
         <v>18</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>27</v>
@@ -5385,37 +5421,37 @@
         <v>6</v>
       </c>
       <c r="J53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K53" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="L53" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M53" s="1">
+        <v>1</v>
+      </c>
+      <c r="N53" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="L53" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M53" s="1">
-        <v>1</v>
-      </c>
-      <c r="N53" s="1" t="s">
+      <c r="O53" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="P53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q53" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="O53" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="P53" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q53" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="R53" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S53" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="U53" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="V53" s="2">
         <v>15.402100000000001</v>
@@ -5441,10 +5477,10 @@
         <v>18</v>
       </c>
       <c r="F54" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>27</v>
@@ -5453,37 +5489,37 @@
         <v>6</v>
       </c>
       <c r="J54" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K54" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="L54" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M54" s="1">
+        <v>1</v>
+      </c>
+      <c r="N54" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="L54" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M54" s="1">
-        <v>1</v>
-      </c>
-      <c r="N54" s="1" t="s">
+      <c r="O54" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q54" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="O54" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="P54" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q54" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="R54" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S54" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="U54" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="V54" s="2">
         <v>15.402100000000001</v>
@@ -5512,7 +5548,7 @@
         <v>25</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>45</v>
+        <v>177</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>27</v>
@@ -5713,10 +5749,10 @@
         <v>4</v>
       </c>
       <c r="F58" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>27</v>
@@ -5755,7 +5791,7 @@
         <v>179</v>
       </c>
       <c r="U58" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="V58" s="2">
         <v>15.400600000000001</v>
@@ -5781,40 +5817,40 @@
         <v>5</v>
       </c>
       <c r="F59" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="H59" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I59" s="1">
+        <v>1</v>
+      </c>
+      <c r="J59" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H59" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I59" s="1">
-        <v>1</v>
-      </c>
-      <c r="J59" s="1" t="s">
+      <c r="K59" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K59" s="1" t="s">
+      <c r="L59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M59" s="1">
+        <v>1</v>
+      </c>
+      <c r="N59" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L59" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M59" s="1">
-        <v>1</v>
-      </c>
-      <c r="N59" s="1" t="s">
+      <c r="O59" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q59" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="O59" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="P59" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q59" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="R59" s="1" t="s">
         <v>35</v>
@@ -5849,40 +5885,40 @@
         <v>5</v>
       </c>
       <c r="F60" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="H60" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I60" s="1">
+        <v>1</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I60" s="1">
-        <v>1</v>
-      </c>
-      <c r="J60" s="1" t="s">
+      <c r="K60" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="L60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M60" s="1">
+        <v>1</v>
+      </c>
+      <c r="N60" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L60" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M60" s="1">
-        <v>1</v>
-      </c>
-      <c r="N60" s="1" t="s">
+      <c r="O60" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q60" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="P60" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q60" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="R60" s="1" t="s">
         <v>35</v>
@@ -5917,40 +5953,40 @@
         <v>5</v>
       </c>
       <c r="F61" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G61" s="1" t="s">
+      <c r="H61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I61" s="1">
+        <v>1</v>
+      </c>
+      <c r="J61" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H61" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I61" s="1">
-        <v>1</v>
-      </c>
-      <c r="J61" s="1" t="s">
+      <c r="K61" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K61" s="1" t="s">
+      <c r="L61" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M61" s="1">
+        <v>1</v>
+      </c>
+      <c r="N61" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L61" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M61" s="1">
-        <v>1</v>
-      </c>
-      <c r="N61" s="1" t="s">
+      <c r="O61" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q61" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="O61" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="P61" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q61" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="R61" s="1" t="s">
         <v>35</v>
@@ -5985,40 +6021,40 @@
         <v>5</v>
       </c>
       <c r="F62" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="H62" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I62" s="1">
+        <v>1</v>
+      </c>
+      <c r="J62" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H62" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I62" s="1">
-        <v>1</v>
-      </c>
-      <c r="J62" s="1" t="s">
+      <c r="K62" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K62" s="1" t="s">
+      <c r="L62" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M62" s="1">
+        <v>1</v>
+      </c>
+      <c r="N62" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L62" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M62" s="1">
-        <v>1</v>
-      </c>
-      <c r="N62" s="1" t="s">
+      <c r="O62" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P62" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q62" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="O62" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="P62" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q62" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="R62" s="1" t="s">
         <v>35</v>
@@ -6503,7 +6539,7 @@
         <v>179</v>
       </c>
       <c r="U69" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="V69" s="2">
         <v>15.401199999999999</v>
@@ -6937,10 +6973,10 @@
         <v>10</v>
       </c>
       <c r="F76" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>27</v>
@@ -6952,7 +6988,7 @@
         <v>219</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>30</v>
@@ -6964,7 +7000,7 @@
         <v>220</v>
       </c>
       <c r="O76" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P76" s="1" t="s">
         <v>33</v>
@@ -7005,10 +7041,10 @@
         <v>10</v>
       </c>
       <c r="F77" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>27</v>
@@ -7073,10 +7109,10 @@
         <v>11</v>
       </c>
       <c r="F78" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G78" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>27</v>
@@ -7141,10 +7177,10 @@
         <v>11</v>
       </c>
       <c r="F79" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>27</v>
@@ -7153,28 +7189,28 @@
         <v>4</v>
       </c>
       <c r="J79" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K79" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K79" s="1" t="s">
+      <c r="L79" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M79" s="1">
+        <v>1</v>
+      </c>
+      <c r="N79" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L79" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M79" s="1">
-        <v>1</v>
-      </c>
-      <c r="N79" s="1" t="s">
+      <c r="O79" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P79" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q79" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="O79" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="P79" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q79" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="R79" s="1" t="s">
         <v>35</v>
@@ -7209,10 +7245,10 @@
         <v>11</v>
       </c>
       <c r="F80" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G80" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>27</v>
@@ -7221,28 +7257,28 @@
         <v>4</v>
       </c>
       <c r="J80" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K80" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K80" s="1" t="s">
+      <c r="L80" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M80" s="1">
+        <v>1</v>
+      </c>
+      <c r="N80" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L80" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M80" s="1">
-        <v>1</v>
-      </c>
-      <c r="N80" s="1" t="s">
+      <c r="O80" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P80" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q80" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="O80" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="P80" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q80" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="R80" s="1" t="s">
         <v>35</v>
@@ -7345,10 +7381,10 @@
         <v>18</v>
       </c>
       <c r="F82" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G82" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>27</v>
@@ -7357,28 +7393,28 @@
         <v>4</v>
       </c>
       <c r="J82" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K82" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K82" s="1" t="s">
+      <c r="L82" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M82" s="1">
+        <v>1</v>
+      </c>
+      <c r="N82" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="L82" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M82" s="1">
-        <v>1</v>
-      </c>
-      <c r="N82" s="1" t="s">
+      <c r="O82" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="P82" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q82" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="O82" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="P82" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q82" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="R82" s="1" t="s">
         <v>35</v>
@@ -7413,10 +7449,10 @@
         <v>18</v>
       </c>
       <c r="F83" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>27</v>
@@ -7425,28 +7461,28 @@
         <v>4</v>
       </c>
       <c r="J83" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K83" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K83" s="1" t="s">
+      <c r="L83" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M83" s="1">
+        <v>1</v>
+      </c>
+      <c r="N83" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="L83" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M83" s="1">
-        <v>1</v>
-      </c>
-      <c r="N83" s="1" t="s">
+      <c r="O83" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="P83" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q83" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="O83" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="P83" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q83" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="R83" s="1" t="s">
         <v>35</v>
@@ -7474,6 +7510,12 @@
       <c r="D84" s="1">
         <v>3</v>
       </c>
+      <c r="E84" s="1">
+        <v>8</v>
+      </c>
+      <c r="F84" s="1">
+        <v>8</v>
+      </c>
       <c r="G84" s="1" t="s">
         <v>246</v>
       </c>
@@ -7486,6 +7528,12 @@
       <c r="L84" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="O84" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P84" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="R84" s="1" t="s">
         <v>35</v>
       </c>
@@ -7515,6 +7563,12 @@
       <c r="D85" s="1">
         <v>3</v>
       </c>
+      <c r="E85" s="1">
+        <v>8</v>
+      </c>
+      <c r="F85" s="1">
+        <v>8</v>
+      </c>
       <c r="G85" s="1" t="s">
         <v>246</v>
       </c>
@@ -7527,6 +7581,12 @@
       <c r="L85" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="O85" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P85" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="R85" s="1" t="s">
         <v>35</v>
       </c>
@@ -7556,6 +7616,12 @@
       <c r="D86" s="1">
         <v>3</v>
       </c>
+      <c r="E86" s="1">
+        <v>7</v>
+      </c>
+      <c r="F86" s="1">
+        <v>7</v>
+      </c>
       <c r="G86" s="1" t="s">
         <v>251</v>
       </c>
@@ -7568,6 +7634,12 @@
       <c r="L86" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="O86" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="P86" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="R86" s="1" t="s">
         <v>35</v>
       </c>
@@ -7597,8 +7669,14 @@
       <c r="D87" s="1">
         <v>3</v>
       </c>
+      <c r="E87" s="1">
+        <v>11</v>
+      </c>
+      <c r="F87" s="1">
+        <v>11</v>
+      </c>
       <c r="G87" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>27</v>
@@ -7609,6 +7687,12 @@
       <c r="L87" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="O87" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="P87" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="R87" s="1" t="s">
         <v>35</v>
       </c>
@@ -7638,17 +7722,29 @@
       <c r="D88" s="1">
         <v>3</v>
       </c>
+      <c r="E88" s="1">
+        <v>5</v>
+      </c>
+      <c r="F88" s="1">
+        <v>5</v>
+      </c>
       <c r="G88" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L88" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="O88" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P88" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="R88" s="1" t="s">
         <v>35</v>
@@ -7679,17 +7775,29 @@
       <c r="D89" s="1">
         <v>3</v>
       </c>
+      <c r="E89" s="1">
+        <v>5</v>
+      </c>
+      <c r="F89" s="1">
+        <v>5</v>
+      </c>
       <c r="G89" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L89" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="O89" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P89" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="R89" s="1" t="s">
         <v>35</v>
@@ -7720,8 +7828,14 @@
       <c r="D90" s="1">
         <v>3</v>
       </c>
+      <c r="E90" s="1">
+        <v>5</v>
+      </c>
+      <c r="F90" s="1">
+        <v>5</v>
+      </c>
       <c r="G90" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>27</v>
@@ -7732,6 +7846,12 @@
       <c r="L90" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="O90" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="P90" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="R90" s="1" t="s">
         <v>35</v>
       </c>
@@ -7761,11 +7881,29 @@
       <c r="D91" s="1">
         <v>3</v>
       </c>
+      <c r="E91" s="1">
+        <v>6</v>
+      </c>
+      <c r="F91" s="1">
+        <v>6</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="H91" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="K91" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="L91" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="O91" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P91" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="R91" s="1" t="s">
         <v>35</v>
@@ -7775,6 +7913,280 @@
       </c>
       <c r="T91" s="1" t="s">
         <v>248</v>
+      </c>
+      <c r="U91" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="V91" s="2">
+        <v>13.303027999999999</v>
+      </c>
+      <c r="W91" s="2">
+        <v>-87.199538000000004</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23">
+      <c r="B92" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D92" s="1">
+        <v>3</v>
+      </c>
+      <c r="E92" s="1">
+        <v>1</v>
+      </c>
+      <c r="F92" s="1">
+        <v>1</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L92" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O92" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P92" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R92" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S92" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="T92" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="U92" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="V92" s="2">
+        <v>15.769266</v>
+      </c>
+      <c r="W92" s="2">
+        <v>-86.808992000000003</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23">
+      <c r="B93" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D93" s="1">
+        <v>3</v>
+      </c>
+      <c r="E93" s="1">
+        <v>4</v>
+      </c>
+      <c r="F93" s="1">
+        <v>4</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="L93" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O93" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="P93" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R93" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S93" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="T93" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="U93" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="V93" s="2">
+        <v>14.768719000000001</v>
+      </c>
+      <c r="W93" s="2">
+        <v>-88.784801000000002</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23">
+      <c r="B94" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D94" s="1">
+        <v>3</v>
+      </c>
+      <c r="E94" s="1">
+        <v>2</v>
+      </c>
+      <c r="F94" s="1">
+        <v>2</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="L94" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O94" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="P94" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R94" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S94" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="T94" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="U94" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="V94" s="2">
+        <v>15.920894000000001</v>
+      </c>
+      <c r="W94" s="2">
+        <v>-85.951768999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23">
+      <c r="B95" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D95" s="1">
+        <v>3</v>
+      </c>
+      <c r="E95" s="1">
+        <v>14</v>
+      </c>
+      <c r="F95" s="1">
+        <v>14</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="L95" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O95" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="P95" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R95" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S95" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="T95" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="U95" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="V95" s="2">
+        <v>14.412167999999999</v>
+      </c>
+      <c r="W95" s="2">
+        <v>-88.956046000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23">
+      <c r="B96" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D96" s="1">
+        <v>3</v>
+      </c>
+      <c r="E96" s="1">
+        <v>17</v>
+      </c>
+      <c r="F96" s="1">
+        <v>17</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O96" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="P96" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R96" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S96" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="T96" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="U96" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="V96" s="2">
+        <v>13.435276</v>
+      </c>
+      <c r="W96" s="2">
+        <v>-87.443899000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-08-2020 03-44-52
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="282" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{521ABC66-966A-4C87-B8EC-72C98C115409}"/>
+  <xr:revisionPtr revIDLastSave="284" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{12574679-8A0F-45EF-AF10-0C691B1E1724}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="270">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -772,9 +772,6 @@
   </si>
   <si>
     <t>Clínica Barrientos Maradiaga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tegucigalpa </t>
   </si>
   <si>
     <t xml:space="preserve">hospital </t>
@@ -1823,8 +1820,8 @@
   <dimension ref="A1:W96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F97" sqref="F97"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G84" sqref="G84:G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -7517,7 +7514,7 @@
         <v>8</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>246</v>
+        <v>39</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>27</v>
@@ -7538,13 +7535,13 @@
         <v>35</v>
       </c>
       <c r="S84" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T84" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="T84" s="1" t="s">
+      <c r="U84" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="U84" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="V84" s="2">
         <v>14.104480000000001</v>
@@ -7570,7 +7567,7 @@
         <v>8</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>246</v>
+        <v>39</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>27</v>
@@ -7591,13 +7588,13 @@
         <v>35</v>
       </c>
       <c r="S85" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T85" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="T85" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="U85" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V85" s="2">
         <v>14.103702999999999</v>
@@ -7623,34 +7620,34 @@
         <v>7</v>
       </c>
       <c r="G86" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K86" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="H86" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K86" s="1" t="s">
+      <c r="L86" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O86" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="P86" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R86" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S86" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T86" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="U86" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="L86" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O86" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="P86" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R86" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S86" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="T86" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="U86" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="V86" s="2">
         <v>13.991413</v>
@@ -7697,13 +7694,13 @@
         <v>35</v>
       </c>
       <c r="S87" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T87" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="T87" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="U87" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="V87" s="2">
         <v>16.317903000000001</v>
@@ -7750,13 +7747,13 @@
         <v>35</v>
       </c>
       <c r="S88" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T88" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="T88" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="U88" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="V88" s="2">
         <v>15.524452999999999</v>
@@ -7803,13 +7800,13 @@
         <v>35</v>
       </c>
       <c r="S89" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T89" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="T89" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="U89" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="V89" s="2">
         <v>15.500176</v>
@@ -7841,28 +7838,28 @@
         <v>27</v>
       </c>
       <c r="K90" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="L90" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O90" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="P90" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R90" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S90" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T90" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="U90" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="L90" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O90" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="P90" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R90" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S90" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="T90" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="U90" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="V90" s="2">
         <v>15.814730000000001</v>
@@ -7909,13 +7906,13 @@
         <v>35</v>
       </c>
       <c r="S91" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T91" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="T91" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="U91" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="V91" s="2">
         <v>13.303027999999999</v>
@@ -7962,13 +7959,13 @@
         <v>35</v>
       </c>
       <c r="S92" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T92" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="T92" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="U92" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="V92" s="2">
         <v>15.769266</v>
@@ -8000,28 +7997,28 @@
         <v>27</v>
       </c>
       <c r="K93" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="L93" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O93" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="P93" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R93" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S93" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T93" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="U93" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="L93" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O93" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="P93" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R93" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S93" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="T93" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="U93" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="V93" s="2">
         <v>14.768719000000001</v>
@@ -8053,28 +8050,28 @@
         <v>27</v>
       </c>
       <c r="K94" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="L94" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O94" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="P94" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R94" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S94" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T94" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="U94" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="L94" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O94" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="P94" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R94" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S94" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="T94" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="U94" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="V94" s="2">
         <v>15.920894000000001</v>
@@ -8100,34 +8097,34 @@
         <v>14</v>
       </c>
       <c r="G95" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K95" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="H95" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K95" s="1" t="s">
+      <c r="L95" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O95" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="P95" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R95" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S95" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T95" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="U95" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="L95" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O95" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="P95" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R95" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S95" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="T95" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="U95" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="V95" s="2">
         <v>14.412167999999999</v>
@@ -8153,34 +8150,34 @@
         <v>17</v>
       </c>
       <c r="G96" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K96" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="H96" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K96" s="1" t="s">
+      <c r="L96" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O96" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="P96" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R96" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S96" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T96" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="U96" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="L96" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O96" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="P96" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R96" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S96" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="T96" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="U96" s="1" t="s">
-        <v>270</v>
       </c>
       <c r="V96" s="2">
         <v>13.435276</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-08-2020 18-46-56
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="329" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0B04FDA8-D53E-4C85-AC3D-150CCD1F347F}"/>
+  <xr:revisionPtr revIDLastSave="418" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{955A1F25-5A4C-4512-B413-A688E2D031E1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="HOSPITALES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$128</definedName>
     <definedName name="_xlnm.Database">HOSPITALES!$A$1:$U$83</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="298">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -874,6 +874,60 @@
   </si>
   <si>
     <t>Hospital San Lorenzo</t>
+  </si>
+  <si>
+    <t>Gracias a Dios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puerto Lempira </t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>Juticalpa</t>
+  </si>
+  <si>
+    <t>Hospital San Francisco</t>
+  </si>
+  <si>
+    <t>Hospital Trochez Montalvan</t>
+  </si>
+  <si>
+    <t>Catacamas</t>
+  </si>
+  <si>
+    <t>Hospital y Clínica Campos</t>
+  </si>
+  <si>
+    <t>Clínica Medicentro</t>
+  </si>
+  <si>
+    <t>Clínica San Lucas</t>
+  </si>
+  <si>
+    <t>Guajiquiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">centro de salud </t>
+  </si>
+  <si>
+    <t>Centro de Salud El Guajiquiro</t>
+  </si>
+  <si>
+    <t>Marcala</t>
+  </si>
+  <si>
+    <t>Centro de Salud Marcala</t>
+  </si>
+  <si>
+    <t>San José</t>
+  </si>
+  <si>
+    <t>Hospital Montecillos</t>
+  </si>
+  <si>
+    <t>Hospiital Roberto Suazo Córdova</t>
   </si>
 </sst>
 </file>
@@ -1526,8 +1580,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W96" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W96" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W128" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W128" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W83">
     <sortCondition ref="S1:S83"/>
   </sortState>
@@ -1857,11 +1911,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W96"/>
+  <dimension ref="A1:W107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="G80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q84" sqref="Q84"/>
+      <pane ySplit="1" topLeftCell="I96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L104" sqref="L104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -8379,6 +8433,220 @@
         <v>-87.443899000000002</v>
       </c>
     </row>
+    <row r="97" spans="7:23">
+      <c r="G97" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="S97" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="U97" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="V97" s="2">
+        <v>15.260996</v>
+      </c>
+      <c r="W97" s="2">
+        <v>-83.778705000000002</v>
+      </c>
+    </row>
+    <row r="98" spans="7:23">
+      <c r="G98" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="S98" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U98" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="V98" s="2">
+        <v>14.665319</v>
+      </c>
+      <c r="W98" s="2">
+        <v>-86.225899999999996</v>
+      </c>
+    </row>
+    <row r="99" spans="7:23">
+      <c r="G99" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="S99" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U99" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="V99" s="2">
+        <v>14.671486</v>
+      </c>
+      <c r="W99" s="2">
+        <v>-86.221147999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="7:23">
+      <c r="G100" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="S100" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U100" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="V100" s="2">
+        <v>14.853908000000001</v>
+      </c>
+      <c r="W100" s="2">
+        <v>-85.894442999999995</v>
+      </c>
+    </row>
+    <row r="101" spans="7:23">
+      <c r="G101" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="S101" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U101" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="V101" s="2">
+        <v>14.851229</v>
+      </c>
+      <c r="W101" s="2">
+        <v>-85.895388999999994</v>
+      </c>
+    </row>
+    <row r="102" spans="7:23">
+      <c r="G102" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="S102" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U102" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="V102" s="2">
+        <v>14.850133</v>
+      </c>
+      <c r="W102" s="2">
+        <v>-85.895661000000004</v>
+      </c>
+    </row>
+    <row r="103" spans="7:23">
+      <c r="G103" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="S103" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="U103" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="V103" s="2">
+        <v>14.120423000000001</v>
+      </c>
+      <c r="W103" s="2">
+        <v>-87.829441000000003</v>
+      </c>
+    </row>
+    <row r="104" spans="7:23">
+      <c r="G104" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="S104" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="U104" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="V104" s="2">
+        <v>14.159074</v>
+      </c>
+      <c r="W104" s="2">
+        <v>-88.036270999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="7:23">
+      <c r="G105" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="S105" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="U105" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V105" s="2">
+        <v>14.248234</v>
+      </c>
+      <c r="W105" s="2">
+        <v>-87.959114999999997</v>
+      </c>
+    </row>
+    <row r="106" spans="7:23">
+      <c r="G106" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="S106" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U106" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="V106" s="2">
+        <v>14.319006</v>
+      </c>
+      <c r="W106" s="2">
+        <v>-87.680940000000007</v>
+      </c>
+    </row>
+    <row r="107" spans="7:23">
+      <c r="S107" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U107" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="V107" s="2">
+        <v>14.322329999999999</v>
+      </c>
+      <c r="W107" s="2">
+        <v>-87.678188000000006</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U83">
     <sortCondition ref="R2:R83"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-08-2020 21-34-23
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="418" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{955A1F25-5A4C-4512-B413-A688E2D031E1}"/>
+  <xr:revisionPtr revIDLastSave="473" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2C9F7B22-2B7B-4853-9AC5-D2A2D67D03EA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="305">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -927,7 +927,28 @@
     <t>Hospital Montecillos</t>
   </si>
   <si>
-    <t>Hospiital Roberto Suazo Córdova</t>
+    <t>Hospital Roberto Suazo Córdova</t>
+  </si>
+  <si>
+    <t>Hospital Regional Santa Teresa</t>
+  </si>
+  <si>
+    <t>Hospital del Valle</t>
+  </si>
+  <si>
+    <t>Hospital Privado de Comayagua</t>
+  </si>
+  <si>
+    <t>La Esperanza</t>
+  </si>
+  <si>
+    <t>Hospital Enrique Aguila Cerrato</t>
+  </si>
+  <si>
+    <t>Tela</t>
+  </si>
+  <si>
+    <t>Hospital Tela Integrado</t>
   </si>
 </sst>
 </file>
@@ -1911,11 +1932,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W107"/>
+  <dimension ref="A1:W113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="I96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L104" sqref="L104"/>
+      <pane ySplit="1" topLeftCell="O101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W115" sqref="W115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -8634,6 +8655,12 @@
       </c>
     </row>
     <row r="107" spans="7:23">
+      <c r="G107" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="S107" s="1" t="s">
         <v>179</v>
       </c>
@@ -8645,6 +8672,126 @@
       </c>
       <c r="W107" s="2">
         <v>-87.678188000000006</v>
+      </c>
+    </row>
+    <row r="108" spans="7:23">
+      <c r="G108" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="S108" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U108" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="V108" s="2">
+        <v>14.453317999999999</v>
+      </c>
+      <c r="W108" s="2">
+        <v>-87.642769000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="7:23">
+      <c r="G109" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="S109" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U109" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="V109" s="2">
+        <v>14.456941</v>
+      </c>
+      <c r="W109" s="2">
+        <v>-87.635479000000004</v>
+      </c>
+    </row>
+    <row r="110" spans="7:23">
+      <c r="G110" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="S110" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U110" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="V110" s="2">
+        <v>14.460008999999999</v>
+      </c>
+      <c r="W110" s="2">
+        <v>-87.638285999999994</v>
+      </c>
+    </row>
+    <row r="111" spans="7:23">
+      <c r="G111" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="S111" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U111" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V111" s="2">
+        <v>14.601864000000001</v>
+      </c>
+      <c r="W111" s="2">
+        <v>-87.844590999999994</v>
+      </c>
+    </row>
+    <row r="112" spans="7:23">
+      <c r="G112" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K112" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="S112" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U112" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="V112" s="2">
+        <v>14.314704000000001</v>
+      </c>
+      <c r="W112" s="2">
+        <v>-88.160505999999998</v>
+      </c>
+    </row>
+    <row r="113" spans="7:23">
+      <c r="G113" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="S113" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U113" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="V113" s="2">
+        <v>15.754151999999999</v>
+      </c>
+      <c r="W113" s="2">
+        <v>-87.489628999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-08-2020 22-55-59
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="473" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2C9F7B22-2B7B-4853-9AC5-D2A2D67D03EA}"/>
+  <xr:revisionPtr revIDLastSave="548" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{651ED0CD-36FC-4866-B335-F8212389BCFD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="318">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -882,7 +882,7 @@
     <t xml:space="preserve">Puerto Lempira </t>
   </si>
   <si>
-    <t>Hospital</t>
+    <t>Hospital Puerto Lempira</t>
   </si>
   <si>
     <t>Juticalpa</t>
@@ -949,6 +949,45 @@
   </si>
   <si>
     <t>Hospital Tela Integrado</t>
+  </si>
+  <si>
+    <t>Cesamo de Ibans</t>
+  </si>
+  <si>
+    <t>Santa Barbará</t>
+  </si>
+  <si>
+    <t>Hospital Santa Barbará Integrado</t>
+  </si>
+  <si>
+    <t>Trinidad</t>
+  </si>
+  <si>
+    <t>Clínica de Emergencia Trinidad</t>
+  </si>
+  <si>
+    <t>Sula</t>
+  </si>
+  <si>
+    <t>Hospital Sula Socorro de lo Atlto</t>
+  </si>
+  <si>
+    <t>Petoa</t>
+  </si>
+  <si>
+    <t>Hospital Luz de Vida</t>
+  </si>
+  <si>
+    <t>Centro Médico Integral de Occidente</t>
+  </si>
+  <si>
+    <t>El Paraíso</t>
+  </si>
+  <si>
+    <t>Centro Médico San Francisco</t>
+  </si>
+  <si>
+    <t>Hospital Alivio del Sufrimiento</t>
   </si>
 </sst>
 </file>
@@ -1932,11 +1971,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W113"/>
+  <dimension ref="A1:W121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="O101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W115" sqref="W115"/>
+      <pane ySplit="1" topLeftCell="P114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W123" sqref="W123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -8468,10 +8507,10 @@
         <v>282</v>
       </c>
       <c r="V97" s="2">
-        <v>15.260996</v>
+        <v>15.265726000000001</v>
       </c>
       <c r="W97" s="2">
-        <v>-83.778705000000002</v>
+        <v>-83.781515999999996</v>
       </c>
     </row>
     <row r="98" spans="7:23">
@@ -8792,6 +8831,163 @@
       </c>
       <c r="W113" s="2">
         <v>-87.489628999999994</v>
+      </c>
+    </row>
+    <row r="114" spans="7:23">
+      <c r="G114" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="S114" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U114" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="V114" s="2">
+        <v>15.908462</v>
+      </c>
+      <c r="W114" s="2">
+        <v>-84.814170000000004</v>
+      </c>
+    </row>
+    <row r="115" spans="7:23">
+      <c r="G115" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="S115" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U115" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="V115" s="2">
+        <v>14.925007000000001</v>
+      </c>
+      <c r="W115" s="2">
+        <v>-88.237927999999997</v>
+      </c>
+    </row>
+    <row r="116" spans="7:23">
+      <c r="G116" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="K116" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S116" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U116" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="V116" s="2">
+        <v>15.143121000000001</v>
+      </c>
+      <c r="W116" s="2">
+        <v>-88.237575000000007</v>
+      </c>
+    </row>
+    <row r="117" spans="7:23">
+      <c r="G117" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="S117" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U117" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="V117" s="2">
+        <v>15.247275</v>
+      </c>
+      <c r="W117" s="2">
+        <v>-88.552238000000003</v>
+      </c>
+    </row>
+    <row r="118" spans="7:23">
+      <c r="G118" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="S118" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U118" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="V118" s="2">
+        <v>15.273072000000001</v>
+      </c>
+      <c r="W118" s="2">
+        <v>-88.284302999999994</v>
+      </c>
+    </row>
+    <row r="119" spans="7:23">
+      <c r="G119" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="S119" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U119" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="V119" s="2">
+        <v>15.348732999999999</v>
+      </c>
+      <c r="W119" s="2">
+        <v>-88.403704000000005</v>
+      </c>
+    </row>
+    <row r="120" spans="7:23">
+      <c r="G120" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="S120" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U120" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="V120" s="2">
+        <v>13.861846</v>
+      </c>
+      <c r="W120" s="2">
+        <v>-86.554258000000004</v>
+      </c>
+    </row>
+    <row r="121" spans="7:23">
+      <c r="G121" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="S121" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U121" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="V121" s="2">
+        <v>13.865371</v>
+      </c>
+      <c r="W121" s="2">
+        <v>-86.562415000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-09-2020 00-16-07
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="548" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{651ED0CD-36FC-4866-B335-F8212389BCFD}"/>
+  <xr:revisionPtr revIDLastSave="550" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BFC16E04-0602-4A76-862B-B5B099E759FB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1974,7 +1974,7 @@
   <dimension ref="A1:W121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="P114" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="N114" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="W123" sqref="W123"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-09-2020 04-16-43
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="550" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BFC16E04-0602-4A76-862B-B5B099E759FB}"/>
+  <xr:revisionPtr revIDLastSave="616" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E4E6C37E-EB1F-441E-84CC-259D2177D584}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="HOSPITALES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$131</definedName>
     <definedName name="_xlnm.Database">HOSPITALES!$A$1:$U$83</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="329">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -480,7 +480,7 @@
     <t>HND-1301</t>
   </si>
   <si>
-    <t>San Lucas</t>
+    <t>Clínica San Lucas</t>
   </si>
   <si>
     <t>1311</t>
@@ -903,9 +903,6 @@
     <t>Clínica Medicentro</t>
   </si>
   <si>
-    <t>Clínica San Lucas</t>
-  </si>
-  <si>
     <t>Guajiquiro</t>
   </si>
   <si>
@@ -988,6 +985,42 @@
   </si>
   <si>
     <t>Hospital Alivio del Sufrimiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yoro </t>
+  </si>
+  <si>
+    <t>Centro de Salud San Antonio Sulaco Yoro</t>
+  </si>
+  <si>
+    <t>Yorito</t>
+  </si>
+  <si>
+    <t>Centro de Salud Yorito</t>
+  </si>
+  <si>
+    <t>Centro de Salud La Sabana</t>
+  </si>
+  <si>
+    <t>Clínica Médica Dra. Chávez</t>
+  </si>
+  <si>
+    <t>Hospital Manuel de Jesus Subirana</t>
+  </si>
+  <si>
+    <t>El Rosario</t>
+  </si>
+  <si>
+    <t>ACTS Clinic</t>
+  </si>
+  <si>
+    <t>Lepaera</t>
+  </si>
+  <si>
+    <t>Centro de Salud Lepaera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cesamo de Santa Cruz </t>
   </si>
 </sst>
 </file>
@@ -1640,8 +1673,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W128" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W128" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W131" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W131" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W83">
     <sortCondition ref="S1:S83"/>
   </sortState>
@@ -1971,11 +2004,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W121"/>
+  <dimension ref="A1:W129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="N114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W123" sqref="W123"/>
+      <pane ySplit="1" topLeftCell="N119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U131" sqref="U131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -8604,7 +8637,7 @@
         <v>72</v>
       </c>
       <c r="U102" s="1" t="s">
-        <v>289</v>
+        <v>148</v>
       </c>
       <c r="V102" s="2">
         <v>14.850133</v>
@@ -8618,13 +8651,13 @@
         <v>63</v>
       </c>
       <c r="K103" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="S103" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="S103" s="1" t="s">
+      <c r="U103" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="U103" s="1" t="s">
-        <v>292</v>
       </c>
       <c r="V103" s="2">
         <v>14.120423000000001</v>
@@ -8638,13 +8671,13 @@
         <v>63</v>
       </c>
       <c r="K104" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="S104" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="U104" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="S104" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="U104" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="V104" s="2">
         <v>14.159074</v>
@@ -8658,10 +8691,10 @@
         <v>63</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="S105" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U105" s="1" t="s">
         <v>44</v>
@@ -8684,7 +8717,7 @@
         <v>179</v>
       </c>
       <c r="U106" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="V106" s="2">
         <v>14.319006</v>
@@ -8704,7 +8737,7 @@
         <v>179</v>
       </c>
       <c r="U107" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="V107" s="2">
         <v>14.322329999999999</v>
@@ -8724,7 +8757,7 @@
         <v>179</v>
       </c>
       <c r="U108" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="V108" s="2">
         <v>14.453317999999999</v>
@@ -8744,7 +8777,7 @@
         <v>179</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V109" s="2">
         <v>14.456941</v>
@@ -8764,7 +8797,7 @@
         <v>179</v>
       </c>
       <c r="U110" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="V110" s="2">
         <v>14.460008999999999</v>
@@ -8798,13 +8831,13 @@
         <v>134</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="S112" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U112" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="V112" s="2">
         <v>14.314704000000001</v>
@@ -8818,13 +8851,13 @@
         <v>26</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="S113" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U113" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="V113" s="2">
         <v>15.754151999999999</v>
@@ -8841,7 +8874,7 @@
         <v>36</v>
       </c>
       <c r="U114" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V114" s="2">
         <v>15.908462</v>
@@ -8852,16 +8885,16 @@
     </row>
     <row r="115" spans="7:23">
       <c r="G115" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="S115" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U115" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="V115" s="2">
         <v>14.925007000000001</v>
@@ -8872,16 +8905,16 @@
     </row>
     <row r="116" spans="7:23">
       <c r="G116" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="S116" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U116" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="V116" s="2">
         <v>15.143121000000001</v>
@@ -8892,16 +8925,16 @@
     </row>
     <row r="117" spans="7:23">
       <c r="G117" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S117" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="V117" s="2">
         <v>15.247275</v>
@@ -8912,16 +8945,16 @@
     </row>
     <row r="118" spans="7:23">
       <c r="G118" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="S118" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U118" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="V118" s="2">
         <v>15.273072000000001</v>
@@ -8932,7 +8965,7 @@
     </row>
     <row r="119" spans="7:23">
       <c r="G119" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>240</v>
@@ -8941,7 +8974,7 @@
         <v>179</v>
       </c>
       <c r="U119" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="V119" s="2">
         <v>15.348732999999999</v>
@@ -8952,16 +8985,16 @@
     </row>
     <row r="120" spans="7:23">
       <c r="G120" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S120" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U120" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="V120" s="2">
         <v>13.861846</v>
@@ -8972,22 +9005,170 @@
     </row>
     <row r="121" spans="7:23">
       <c r="G121" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S121" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U121" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="V121" s="2">
         <v>13.865371</v>
       </c>
       <c r="W121" s="2">
         <v>-86.562415000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="7:23">
+      <c r="G122" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="S122" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U122" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="V122" s="2">
+        <v>14.985823</v>
+      </c>
+      <c r="W122" s="2">
+        <v>-87.294527000000002</v>
+      </c>
+    </row>
+    <row r="123" spans="7:23">
+      <c r="G123" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K123" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="S123" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U123" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="V123" s="2">
+        <v>15.065429</v>
+      </c>
+      <c r="W123" s="2">
+        <v>-87.277242999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="7:23">
+      <c r="G124" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="S124" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U124" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="V124" s="2">
+        <v>15.108616</v>
+      </c>
+      <c r="W124" s="2">
+        <v>-87.280530999999996</v>
+      </c>
+    </row>
+    <row r="125" spans="7:23">
+      <c r="G125" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="S125" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U125" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="V125" s="2">
+        <v>15.137855999999999</v>
+      </c>
+      <c r="W125" s="2">
+        <v>-87.125667000000007</v>
+      </c>
+    </row>
+    <row r="126" spans="7:23">
+      <c r="G126" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="S126" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U126" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="V126" s="2">
+        <v>15.137337</v>
+      </c>
+      <c r="W126" s="2">
+        <v>-87.133142000000007</v>
+      </c>
+    </row>
+    <row r="127" spans="7:23">
+      <c r="G127" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="S127" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U127" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="V127" s="2">
+        <v>15.276194</v>
+      </c>
+      <c r="W127" s="2">
+        <v>-87.324967999999998</v>
+      </c>
+    </row>
+    <row r="128" spans="7:23">
+      <c r="G128" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="S128" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U128" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="V128" s="2">
+        <v>14.780340000000001</v>
+      </c>
+      <c r="W128" s="2">
+        <v>-88.588606999999996</v>
+      </c>
+    </row>
+    <row r="129" spans="19:23">
+      <c r="S129" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U129" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="V129" s="2">
+        <v>14.329539</v>
+      </c>
+      <c r="W129" s="2">
+        <v>-88.522634999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-09-2020 05-37-52
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="616" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E4E6C37E-EB1F-441E-84CC-259D2177D584}"/>
+  <xr:revisionPtr revIDLastSave="668" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F71B3D90-C4B7-4873-AB29-5C06961016F4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="HOSPITALES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$139</definedName>
     <definedName name="_xlnm.Database">HOSPITALES!$A$1:$U$83</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="339">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -1020,7 +1020,37 @@
     <t>Centro de Salud Lepaera</t>
   </si>
   <si>
+    <t>Santa Cruz</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cesamo de Santa Cruz </t>
+  </si>
+  <si>
+    <t>Gualcinse</t>
+  </si>
+  <si>
+    <t>Hospital del Sur Dr. Lempira</t>
+  </si>
+  <si>
+    <t>Nacaome</t>
+  </si>
+  <si>
+    <t>Policlínica Nacaome</t>
+  </si>
+  <si>
+    <t>Centro Médico Juárez</t>
+  </si>
+  <si>
+    <t>Langue</t>
+  </si>
+  <si>
+    <t>Centro de Salud de Langue</t>
+  </si>
+  <si>
+    <t>Guascorán</t>
+  </si>
+  <si>
+    <t>Medicenter</t>
   </si>
 </sst>
 </file>
@@ -1673,8 +1703,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W131" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W131" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W139" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W139" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W83">
     <sortCondition ref="S1:S83"/>
   </sortState>
@@ -2004,11 +2034,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W129"/>
+  <dimension ref="A1:W135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="N119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U131" sqref="U131"/>
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D96" sqref="D96:D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -8526,7 +8556,16 @@
         <v>-87.443899000000002</v>
       </c>
     </row>
-    <row r="97" spans="7:23">
+    <row r="97" spans="2:23">
+      <c r="B97" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D97" s="1">
+        <v>3</v>
+      </c>
       <c r="G97" s="1" t="s">
         <v>280</v>
       </c>
@@ -8546,7 +8585,16 @@
         <v>-83.781515999999996</v>
       </c>
     </row>
-    <row r="98" spans="7:23">
+    <row r="98" spans="2:23">
+      <c r="B98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D98" s="1">
+        <v>3</v>
+      </c>
       <c r="G98" s="1" t="s">
         <v>155</v>
       </c>
@@ -8566,7 +8614,16 @@
         <v>-86.225899999999996</v>
       </c>
     </row>
-    <row r="99" spans="7:23">
+    <row r="99" spans="2:23">
+      <c r="B99" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D99" s="1">
+        <v>3</v>
+      </c>
       <c r="G99" s="1" t="s">
         <v>155</v>
       </c>
@@ -8586,7 +8643,16 @@
         <v>-86.221147999999999</v>
       </c>
     </row>
-    <row r="100" spans="7:23">
+    <row r="100" spans="2:23">
+      <c r="B100" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D100" s="1">
+        <v>3</v>
+      </c>
       <c r="G100" s="1" t="s">
         <v>155</v>
       </c>
@@ -8606,7 +8672,16 @@
         <v>-85.894442999999995</v>
       </c>
     </row>
-    <row r="101" spans="7:23">
+    <row r="101" spans="2:23">
+      <c r="B101" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D101" s="1">
+        <v>3</v>
+      </c>
       <c r="G101" s="1" t="s">
         <v>155</v>
       </c>
@@ -8626,7 +8701,16 @@
         <v>-85.895388999999994</v>
       </c>
     </row>
-    <row r="102" spans="7:23">
+    <row r="102" spans="2:23">
+      <c r="B102" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D102" s="1">
+        <v>3</v>
+      </c>
       <c r="G102" s="1" t="s">
         <v>155</v>
       </c>
@@ -8646,7 +8730,16 @@
         <v>-85.895661000000004</v>
       </c>
     </row>
-    <row r="103" spans="7:23">
+    <row r="103" spans="2:23">
+      <c r="B103" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D103" s="1">
+        <v>3</v>
+      </c>
       <c r="G103" s="1" t="s">
         <v>63</v>
       </c>
@@ -8666,7 +8759,16 @@
         <v>-87.829441000000003</v>
       </c>
     </row>
-    <row r="104" spans="7:23">
+    <row r="104" spans="2:23">
+      <c r="B104" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D104" s="1">
+        <v>3</v>
+      </c>
       <c r="G104" s="1" t="s">
         <v>63</v>
       </c>
@@ -8686,7 +8788,16 @@
         <v>-88.036270999999999</v>
       </c>
     </row>
-    <row r="105" spans="7:23">
+    <row r="105" spans="2:23">
+      <c r="B105" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D105" s="1">
+        <v>3</v>
+      </c>
       <c r="G105" s="1" t="s">
         <v>63</v>
       </c>
@@ -8706,7 +8817,16 @@
         <v>-87.959114999999997</v>
       </c>
     </row>
-    <row r="106" spans="7:23">
+    <row r="106" spans="2:23">
+      <c r="B106" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D106" s="1">
+        <v>3</v>
+      </c>
       <c r="G106" s="1" t="s">
         <v>63</v>
       </c>
@@ -8726,7 +8846,16 @@
         <v>-87.680940000000007</v>
       </c>
     </row>
-    <row r="107" spans="7:23">
+    <row r="107" spans="2:23">
+      <c r="B107" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D107" s="1">
+        <v>3</v>
+      </c>
       <c r="G107" s="1" t="s">
         <v>63</v>
       </c>
@@ -8746,7 +8875,16 @@
         <v>-87.678188000000006</v>
       </c>
     </row>
-    <row r="108" spans="7:23">
+    <row r="108" spans="2:23">
+      <c r="B108" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D108" s="1">
+        <v>3</v>
+      </c>
       <c r="G108" s="1" t="s">
         <v>189</v>
       </c>
@@ -8766,7 +8904,16 @@
         <v>-87.642769000000001</v>
       </c>
     </row>
-    <row r="109" spans="7:23">
+    <row r="109" spans="2:23">
+      <c r="B109" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D109" s="1">
+        <v>3</v>
+      </c>
       <c r="G109" s="1" t="s">
         <v>189</v>
       </c>
@@ -8786,7 +8933,16 @@
         <v>-87.635479000000004</v>
       </c>
     </row>
-    <row r="110" spans="7:23">
+    <row r="110" spans="2:23">
+      <c r="B110" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D110" s="1">
+        <v>3</v>
+      </c>
       <c r="G110" s="1" t="s">
         <v>189</v>
       </c>
@@ -8806,7 +8962,16 @@
         <v>-87.638285999999994</v>
       </c>
     </row>
-    <row r="111" spans="7:23">
+    <row r="111" spans="2:23">
+      <c r="B111" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D111" s="1">
+        <v>3</v>
+      </c>
       <c r="G111" s="1" t="s">
         <v>189</v>
       </c>
@@ -8826,7 +8991,16 @@
         <v>-87.844590999999994</v>
       </c>
     </row>
-    <row r="112" spans="7:23">
+    <row r="112" spans="2:23">
+      <c r="B112" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D112" s="1">
+        <v>3</v>
+      </c>
       <c r="G112" s="1" t="s">
         <v>134</v>
       </c>
@@ -8846,7 +9020,16 @@
         <v>-88.160505999999998</v>
       </c>
     </row>
-    <row r="113" spans="7:23">
+    <row r="113" spans="2:23">
+      <c r="B113" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D113" s="1">
+        <v>3</v>
+      </c>
       <c r="G113" s="1" t="s">
         <v>26</v>
       </c>
@@ -8866,7 +9049,16 @@
         <v>-87.489628999999994</v>
       </c>
     </row>
-    <row r="114" spans="7:23">
+    <row r="114" spans="2:23">
+      <c r="B114" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D114" s="1">
+        <v>3</v>
+      </c>
       <c r="G114" s="1" t="s">
         <v>280</v>
       </c>
@@ -8883,7 +9075,16 @@
         <v>-84.814170000000004</v>
       </c>
     </row>
-    <row r="115" spans="7:23">
+    <row r="115" spans="2:23">
+      <c r="B115" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D115" s="1">
+        <v>3</v>
+      </c>
       <c r="G115" s="1" t="s">
         <v>305</v>
       </c>
@@ -8903,7 +9104,16 @@
         <v>-88.237927999999997</v>
       </c>
     </row>
-    <row r="116" spans="7:23">
+    <row r="116" spans="2:23">
+      <c r="B116" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D116" s="1">
+        <v>3</v>
+      </c>
       <c r="G116" s="1" t="s">
         <v>305</v>
       </c>
@@ -8923,7 +9133,16 @@
         <v>-88.237575000000007</v>
       </c>
     </row>
-    <row r="117" spans="7:23">
+    <row r="117" spans="2:23">
+      <c r="B117" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D117" s="1">
+        <v>3</v>
+      </c>
       <c r="G117" s="1" t="s">
         <v>305</v>
       </c>
@@ -8943,7 +9162,16 @@
         <v>-88.552238000000003</v>
       </c>
     </row>
-    <row r="118" spans="7:23">
+    <row r="118" spans="2:23">
+      <c r="B118" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D118" s="1">
+        <v>3</v>
+      </c>
       <c r="G118" s="1" t="s">
         <v>305</v>
       </c>
@@ -8963,7 +9191,16 @@
         <v>-88.284302999999994</v>
       </c>
     </row>
-    <row r="119" spans="7:23">
+    <row r="119" spans="2:23">
+      <c r="B119" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D119" s="1">
+        <v>3</v>
+      </c>
       <c r="G119" s="1" t="s">
         <v>305</v>
       </c>
@@ -8983,7 +9220,16 @@
         <v>-88.403704000000005</v>
       </c>
     </row>
-    <row r="120" spans="7:23">
+    <row r="120" spans="2:23">
+      <c r="B120" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D120" s="1">
+        <v>3</v>
+      </c>
       <c r="G120" s="1" t="s">
         <v>314</v>
       </c>
@@ -9003,7 +9249,16 @@
         <v>-86.554258000000004</v>
       </c>
     </row>
-    <row r="121" spans="7:23">
+    <row r="121" spans="2:23">
+      <c r="B121" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D121" s="1">
+        <v>3</v>
+      </c>
       <c r="G121" s="1" t="s">
         <v>314</v>
       </c>
@@ -9023,7 +9278,16 @@
         <v>-86.562415000000001</v>
       </c>
     </row>
-    <row r="122" spans="7:23">
+    <row r="122" spans="2:23">
+      <c r="B122" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D122" s="1">
+        <v>3</v>
+      </c>
       <c r="G122" s="1" t="s">
         <v>317</v>
       </c>
@@ -9040,7 +9304,16 @@
         <v>-87.294527000000002</v>
       </c>
     </row>
-    <row r="123" spans="7:23">
+    <row r="123" spans="2:23">
+      <c r="B123" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D123" s="1">
+        <v>3</v>
+      </c>
       <c r="G123" s="1" t="s">
         <v>162</v>
       </c>
@@ -9060,7 +9333,16 @@
         <v>-87.277242999999999</v>
       </c>
     </row>
-    <row r="124" spans="7:23">
+    <row r="124" spans="2:23">
+      <c r="B124" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D124" s="1">
+        <v>3</v>
+      </c>
       <c r="G124" s="1" t="s">
         <v>162</v>
       </c>
@@ -9077,7 +9359,16 @@
         <v>-87.280530999999996</v>
       </c>
     </row>
-    <row r="125" spans="7:23">
+    <row r="125" spans="2:23">
+      <c r="B125" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D125" s="1">
+        <v>3</v>
+      </c>
       <c r="G125" s="1" t="s">
         <v>162</v>
       </c>
@@ -9097,7 +9388,16 @@
         <v>-87.125667000000007</v>
       </c>
     </row>
-    <row r="126" spans="7:23">
+    <row r="126" spans="2:23">
+      <c r="B126" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D126" s="1">
+        <v>3</v>
+      </c>
       <c r="G126" s="1" t="s">
         <v>162</v>
       </c>
@@ -9117,7 +9417,16 @@
         <v>-87.133142000000007</v>
       </c>
     </row>
-    <row r="127" spans="7:23">
+    <row r="127" spans="2:23">
+      <c r="B127" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D127" s="1">
+        <v>3</v>
+      </c>
       <c r="G127" s="1" t="s">
         <v>162</v>
       </c>
@@ -9137,7 +9446,16 @@
         <v>-87.324967999999998</v>
       </c>
     </row>
-    <row r="128" spans="7:23">
+    <row r="128" spans="2:23">
+      <c r="B128" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D128" s="1">
+        <v>3</v>
+      </c>
       <c r="G128" s="1" t="s">
         <v>143</v>
       </c>
@@ -9157,18 +9475,204 @@
         <v>-88.588606999999996</v>
       </c>
     </row>
-    <row r="129" spans="19:23">
+    <row r="129" spans="2:23">
+      <c r="B129" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D129" s="1">
+        <v>3</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="S129" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="V129" s="2">
         <v>14.329539</v>
       </c>
       <c r="W129" s="2">
         <v>-88.522634999999994</v>
+      </c>
+    </row>
+    <row r="130" spans="2:23">
+      <c r="B130" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D130" s="1">
+        <v>3</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K130" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="S130" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U130" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="V130" s="2">
+        <v>14.126211</v>
+      </c>
+      <c r="W130" s="2">
+        <v>-88.543222999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="2:23">
+      <c r="B131" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D131" s="1">
+        <v>3</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="S131" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U131" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V131" s="2">
+        <v>14.114020999999999</v>
+      </c>
+      <c r="W131" s="2">
+        <v>-88.651722000000007</v>
+      </c>
+    </row>
+    <row r="132" spans="2:23">
+      <c r="B132" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D132" s="1">
+        <v>3</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K132" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="S132" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U132" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="V132" s="2">
+        <v>13.530787999999999</v>
+      </c>
+      <c r="W132" s="2">
+        <v>-87.498217999999994</v>
+      </c>
+    </row>
+    <row r="133" spans="2:23">
+      <c r="B133" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D133" s="1">
+        <v>3</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K133" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="S133" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U133" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="V133" s="2">
+        <v>13.532709000000001</v>
+      </c>
+      <c r="W133" s="2">
+        <v>-87.492543999999995</v>
+      </c>
+    </row>
+    <row r="134" spans="2:23">
+      <c r="B134" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D134" s="1">
+        <v>3</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K134" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="S134" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U134" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="V134" s="2">
+        <v>13.62003</v>
+      </c>
+      <c r="W134" s="2">
+        <v>-87.657388999999995</v>
+      </c>
+    </row>
+    <row r="135" spans="2:23">
+      <c r="B135" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D135" s="1">
+        <v>3</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K135" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="S135" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U135" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="V135" s="2">
+        <v>13.610545</v>
+      </c>
+      <c r="W135" s="2">
+        <v>-87.752651</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-10-2020 03-14-52
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="668" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F71B3D90-C4B7-4873-AB29-5C06961016F4}"/>
+  <xr:revisionPtr revIDLastSave="723" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{529982E2-1FFC-4553-902F-04259DCB81D4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="353">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -876,6 +876,9 @@
     <t>Hospital San Lorenzo</t>
   </si>
   <si>
+    <t>09</t>
+  </si>
+  <si>
     <t>Gracias a Dios</t>
   </si>
   <si>
@@ -885,6 +888,9 @@
     <t>Hospital Puerto Lempira</t>
   </si>
   <si>
+    <t>1501</t>
+  </si>
+  <si>
     <t>Juticalpa</t>
   </si>
   <si>
@@ -894,6 +900,9 @@
     <t>Hospital Trochez Montalvan</t>
   </si>
   <si>
+    <t>1503</t>
+  </si>
+  <si>
     <t>Catacamas</t>
   </si>
   <si>
@@ -954,21 +963,27 @@
     <t>Santa Barbará</t>
   </si>
   <si>
+    <t>1601</t>
+  </si>
+  <si>
     <t>Hospital Santa Barbará Integrado</t>
   </si>
   <si>
+    <t>1626</t>
+  </si>
+  <si>
     <t>Trinidad</t>
   </si>
   <si>
     <t>Clínica de Emergencia Trinidad</t>
   </si>
   <si>
-    <t>Sula</t>
-  </si>
-  <si>
     <t>Hospital Sula Socorro de lo Atlto</t>
   </si>
   <si>
+    <t>1615</t>
+  </si>
+  <si>
     <t>Petoa</t>
   </si>
   <si>
@@ -978,6 +993,9 @@
     <t>Centro Médico Integral de Occidente</t>
   </si>
   <si>
+    <t>07</t>
+  </si>
+  <si>
     <t>El Paraíso</t>
   </si>
   <si>
@@ -993,6 +1011,9 @@
     <t>Centro de Salud San Antonio Sulaco Yoro</t>
   </si>
   <si>
+    <t>1811</t>
+  </si>
+  <si>
     <t>Yorito</t>
   </si>
   <si>
@@ -1002,36 +1023,51 @@
     <t>Centro de Salud La Sabana</t>
   </si>
   <si>
+    <t>1801</t>
+  </si>
+  <si>
     <t>Clínica Médica Dra. Chávez</t>
   </si>
   <si>
     <t>Hospital Manuel de Jesus Subirana</t>
   </si>
   <si>
-    <t>El Rosario</t>
-  </si>
-  <si>
     <t>ACTS Clinic</t>
   </si>
   <si>
+    <t>1313</t>
+  </si>
+  <si>
     <t>Lepaera</t>
   </si>
   <si>
     <t>Centro de Salud Lepaera</t>
   </si>
   <si>
+    <t>1322</t>
+  </si>
+  <si>
     <t>Santa Cruz</t>
   </si>
   <si>
     <t xml:space="preserve">Cesamo de Santa Cruz </t>
   </si>
   <si>
+    <t>1306</t>
+  </si>
+  <si>
     <t>Gualcinse</t>
   </si>
   <si>
     <t>Hospital del Sur Dr. Lempira</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>1701</t>
+  </si>
+  <si>
     <t>Nacaome</t>
   </si>
   <si>
@@ -1041,13 +1077,19 @@
     <t>Centro Médico Juárez</t>
   </si>
   <si>
+    <t>1707</t>
+  </si>
+  <si>
     <t>Langue</t>
   </si>
   <si>
     <t>Centro de Salud de Langue</t>
   </si>
   <si>
-    <t>Guascorán</t>
+    <t>1706</t>
+  </si>
+  <si>
+    <t>Goascorán</t>
   </si>
   <si>
     <t>Medicenter</t>
@@ -1377,7 +1419,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1501,6 +1543,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1546,7 +1599,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1555,6 +1608,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2037,8 +2091,8 @@
   <dimension ref="A1:W135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D96" sqref="D96:D135"/>
+      <pane ySplit="1" topLeftCell="F114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -8556,7 +8610,7 @@
         <v>-87.443899000000002</v>
       </c>
     </row>
-    <row r="97" spans="2:23">
+    <row r="97" spans="2:23" ht="15">
       <c r="B97" s="1" t="s">
         <v>23</v>
       </c>
@@ -8566,17 +8620,26 @@
       <c r="D97" s="1">
         <v>3</v>
       </c>
+      <c r="E97" s="7">
+        <v>9</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>280</v>
+      </c>
       <c r="G97" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="S97" s="1" t="s">
         <v>246</v>
       </c>
       <c r="U97" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="V97" s="2">
         <v>15.265726000000001</v>
@@ -8585,7 +8648,7 @@
         <v>-83.781515999999996</v>
       </c>
     </row>
-    <row r="98" spans="2:23">
+    <row r="98" spans="2:23" ht="15">
       <c r="B98" s="1" t="s">
         <v>23</v>
       </c>
@@ -8594,18 +8657,33 @@
       </c>
       <c r="D98" s="1">
         <v>3</v>
+      </c>
+      <c r="E98" s="7">
+        <v>15</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="H98" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I98" s="7">
+        <v>1</v>
+      </c>
+      <c r="J98" s="7" t="s">
+        <v>284</v>
+      </c>
       <c r="K98" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="S98" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U98" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="V98" s="2">
         <v>14.665319</v>
@@ -8614,7 +8692,7 @@
         <v>-86.225899999999996</v>
       </c>
     </row>
-    <row r="99" spans="2:23">
+    <row r="99" spans="2:23" ht="15">
       <c r="B99" s="1" t="s">
         <v>23</v>
       </c>
@@ -8623,18 +8701,33 @@
       </c>
       <c r="D99" s="1">
         <v>3</v>
+      </c>
+      <c r="E99" s="7">
+        <v>15</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="H99" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I99" s="7">
+        <v>1</v>
+      </c>
+      <c r="J99" s="7" t="s">
+        <v>284</v>
+      </c>
       <c r="K99" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="S99" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U99" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="V99" s="2">
         <v>14.671486</v>
@@ -8643,7 +8736,7 @@
         <v>-86.221147999999999</v>
       </c>
     </row>
-    <row r="100" spans="2:23">
+    <row r="100" spans="2:23" ht="15">
       <c r="B100" s="1" t="s">
         <v>23</v>
       </c>
@@ -8652,18 +8745,33 @@
       </c>
       <c r="D100" s="1">
         <v>3</v>
+      </c>
+      <c r="E100" s="7">
+        <v>15</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="H100" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I100" s="7">
+        <v>3</v>
+      </c>
+      <c r="J100" s="7" t="s">
+        <v>288</v>
+      </c>
       <c r="K100" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="S100" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U100" s="1" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="V100" s="2">
         <v>14.853908000000001</v>
@@ -8672,7 +8780,7 @@
         <v>-85.894442999999995</v>
       </c>
     </row>
-    <row r="101" spans="2:23">
+    <row r="101" spans="2:23" ht="15">
       <c r="B101" s="1" t="s">
         <v>23</v>
       </c>
@@ -8681,18 +8789,33 @@
       </c>
       <c r="D101" s="1">
         <v>3</v>
+      </c>
+      <c r="E101" s="7">
+        <v>15</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="H101" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I101" s="7">
+        <v>3</v>
+      </c>
+      <c r="J101" s="7" t="s">
+        <v>288</v>
+      </c>
       <c r="K101" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="S101" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U101" s="1" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="V101" s="2">
         <v>14.851229</v>
@@ -8701,7 +8824,7 @@
         <v>-85.895388999999994</v>
       </c>
     </row>
-    <row r="102" spans="2:23">
+    <row r="102" spans="2:23" ht="15">
       <c r="B102" s="1" t="s">
         <v>23</v>
       </c>
@@ -8710,12 +8833,27 @@
       </c>
       <c r="D102" s="1">
         <v>3</v>
+      </c>
+      <c r="E102" s="7">
+        <v>15</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="H102" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" s="7">
+        <v>3</v>
+      </c>
+      <c r="J102" s="7" t="s">
+        <v>288</v>
+      </c>
       <c r="K102" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="S102" s="1" t="s">
         <v>72</v>
@@ -8730,7 +8868,7 @@
         <v>-85.895661000000004</v>
       </c>
     </row>
-    <row r="103" spans="2:23">
+    <row r="103" spans="2:23" ht="15">
       <c r="B103" s="1" t="s">
         <v>23</v>
       </c>
@@ -8739,18 +8877,27 @@
       </c>
       <c r="D103" s="1">
         <v>3</v>
+      </c>
+      <c r="E103" s="7">
+        <v>12</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="H103" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K103" s="1" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="S103" s="1" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="U103" s="1" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="V103" s="2">
         <v>14.120423000000001</v>
@@ -8759,7 +8906,7 @@
         <v>-87.829441000000003</v>
       </c>
     </row>
-    <row r="104" spans="2:23">
+    <row r="104" spans="2:23" ht="15">
       <c r="B104" s="1" t="s">
         <v>23</v>
       </c>
@@ -8768,18 +8915,27 @@
       </c>
       <c r="D104" s="1">
         <v>3</v>
+      </c>
+      <c r="E104" s="7">
+        <v>12</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="H104" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K104" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="S104" s="1" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="U104" s="1" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="V104" s="2">
         <v>14.159074</v>
@@ -8798,14 +8954,23 @@
       <c r="D105" s="1">
         <v>3</v>
       </c>
+      <c r="E105" s="7">
+        <v>12</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="G105" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="H105" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K105" s="1" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="S105" s="1" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="U105" s="1" t="s">
         <v>44</v>
@@ -8827,9 +8992,18 @@
       <c r="D106" s="1">
         <v>3</v>
       </c>
+      <c r="E106" s="7">
+        <v>12</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="G106" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="H106" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K106" s="1" t="s">
         <v>63</v>
       </c>
@@ -8837,7 +9011,7 @@
         <v>179</v>
       </c>
       <c r="U106" s="1" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="V106" s="2">
         <v>14.319006</v>
@@ -8856,9 +9030,18 @@
       <c r="D107" s="1">
         <v>3</v>
       </c>
+      <c r="E107" s="7">
+        <v>12</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="G107" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="H107" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K107" s="1" t="s">
         <v>63</v>
       </c>
@@ -8866,7 +9049,7 @@
         <v>179</v>
       </c>
       <c r="U107" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="V107" s="2">
         <v>14.322329999999999</v>
@@ -8875,7 +9058,7 @@
         <v>-87.678188000000006</v>
       </c>
     </row>
-    <row r="108" spans="2:23">
+    <row r="108" spans="2:23" ht="15">
       <c r="B108" s="1" t="s">
         <v>23</v>
       </c>
@@ -8884,10 +9067,19 @@
       </c>
       <c r="D108" s="1">
         <v>3</v>
+      </c>
+      <c r="E108" s="7">
+        <v>3</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="H108" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K108" s="1" t="s">
         <v>189</v>
       </c>
@@ -8895,7 +9087,7 @@
         <v>179</v>
       </c>
       <c r="U108" s="1" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="V108" s="2">
         <v>14.453317999999999</v>
@@ -8904,7 +9096,7 @@
         <v>-87.642769000000001</v>
       </c>
     </row>
-    <row r="109" spans="2:23">
+    <row r="109" spans="2:23" ht="15">
       <c r="B109" s="1" t="s">
         <v>23</v>
       </c>
@@ -8913,10 +9105,19 @@
       </c>
       <c r="D109" s="1">
         <v>3</v>
+      </c>
+      <c r="E109" s="7">
+        <v>3</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="H109" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K109" s="1" t="s">
         <v>189</v>
       </c>
@@ -8924,7 +9125,7 @@
         <v>179</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="V109" s="2">
         <v>14.456941</v>
@@ -8943,9 +9144,18 @@
       <c r="D110" s="1">
         <v>3</v>
       </c>
+      <c r="E110" s="7">
+        <v>3</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>188</v>
+      </c>
       <c r="G110" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="H110" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K110" s="1" t="s">
         <v>189</v>
       </c>
@@ -8953,7 +9163,7 @@
         <v>179</v>
       </c>
       <c r="U110" s="1" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="V110" s="2">
         <v>14.460008999999999</v>
@@ -8972,9 +9182,18 @@
       <c r="D111" s="1">
         <v>3</v>
       </c>
+      <c r="E111" s="7">
+        <v>3</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>188</v>
+      </c>
       <c r="G111" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="H111" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K111" s="1" t="s">
         <v>191</v>
       </c>
@@ -8991,7 +9210,7 @@
         <v>-87.844590999999994</v>
       </c>
     </row>
-    <row r="112" spans="2:23">
+    <row r="112" spans="2:23" ht="15">
       <c r="B112" s="1" t="s">
         <v>23</v>
       </c>
@@ -9000,18 +9219,27 @@
       </c>
       <c r="D112" s="1">
         <v>3</v>
+      </c>
+      <c r="E112" s="7">
+        <v>10</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>134</v>
       </c>
+      <c r="H112" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K112" s="1" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="S112" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U112" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="V112" s="2">
         <v>14.314704000000001</v>
@@ -9020,7 +9248,7 @@
         <v>-88.160505999999998</v>
       </c>
     </row>
-    <row r="113" spans="2:23">
+    <row r="113" spans="2:23" ht="15">
       <c r="B113" s="1" t="s">
         <v>23</v>
       </c>
@@ -9029,18 +9257,27 @@
       </c>
       <c r="D113" s="1">
         <v>3</v>
+      </c>
+      <c r="E113" s="7">
+        <v>1</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H113" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K113" s="1" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="S113" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U113" s="1" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="V113" s="2">
         <v>15.754151999999999</v>
@@ -9049,7 +9286,7 @@
         <v>-87.489628999999994</v>
       </c>
     </row>
-    <row r="114" spans="2:23">
+    <row r="114" spans="2:23" ht="15">
       <c r="B114" s="1" t="s">
         <v>23</v>
       </c>
@@ -9059,14 +9296,23 @@
       <c r="D114" s="1">
         <v>3</v>
       </c>
+      <c r="E114" s="7">
+        <v>9</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>280</v>
+      </c>
       <c r="G114" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="S114" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U114" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="V114" s="2">
         <v>15.908462</v>
@@ -9075,7 +9321,7 @@
         <v>-84.814170000000004</v>
       </c>
     </row>
-    <row r="115" spans="2:23">
+    <row r="115" spans="2:23" ht="15">
       <c r="B115" s="1" t="s">
         <v>23</v>
       </c>
@@ -9085,17 +9331,32 @@
       <c r="D115" s="1">
         <v>3</v>
       </c>
+      <c r="E115" s="7">
+        <v>16</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>237</v>
+      </c>
       <c r="G115" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I115" s="7">
+        <v>1</v>
+      </c>
+      <c r="J115" s="7" t="s">
+        <v>309</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="S115" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U115" s="1" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="V115" s="2">
         <v>14.925007000000001</v>
@@ -9104,7 +9365,7 @@
         <v>-88.237927999999997</v>
       </c>
     </row>
-    <row r="116" spans="2:23">
+    <row r="116" spans="2:23" ht="15">
       <c r="B116" s="1" t="s">
         <v>23</v>
       </c>
@@ -9114,17 +9375,32 @@
       <c r="D116" s="1">
         <v>3</v>
       </c>
+      <c r="E116" s="7">
+        <v>16</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>237</v>
+      </c>
       <c r="G116" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" s="7">
+        <v>26</v>
+      </c>
+      <c r="J116" s="7" t="s">
+        <v>311</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="S116" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U116" s="1" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="V116" s="2">
         <v>15.143121000000001</v>
@@ -9143,17 +9419,23 @@
       <c r="D117" s="1">
         <v>3</v>
       </c>
+      <c r="E117" s="7">
+        <v>16</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>237</v>
+      </c>
       <c r="G117" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="K117" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="S117" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="V117" s="2">
         <v>15.247275</v>
@@ -9162,7 +9444,7 @@
         <v>-88.552238000000003</v>
       </c>
     </row>
-    <row r="118" spans="2:23">
+    <row r="118" spans="2:23" ht="15">
       <c r="B118" s="1" t="s">
         <v>23</v>
       </c>
@@ -9172,17 +9454,32 @@
       <c r="D118" s="1">
         <v>3</v>
       </c>
+      <c r="E118" s="7">
+        <v>16</v>
+      </c>
+      <c r="F118" s="7" t="s">
+        <v>237</v>
+      </c>
       <c r="G118" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I118" s="7">
+        <v>15</v>
+      </c>
+      <c r="J118" s="7" t="s">
+        <v>315</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="S118" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U118" s="1" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="V118" s="2">
         <v>15.273072000000001</v>
@@ -9191,7 +9488,7 @@
         <v>-88.284302999999994</v>
       </c>
     </row>
-    <row r="119" spans="2:23">
+    <row r="119" spans="2:23" ht="15">
       <c r="B119" s="1" t="s">
         <v>23</v>
       </c>
@@ -9201,8 +9498,23 @@
       <c r="D119" s="1">
         <v>3</v>
       </c>
+      <c r="E119" s="7">
+        <v>16</v>
+      </c>
+      <c r="F119" s="7" t="s">
+        <v>237</v>
+      </c>
       <c r="G119" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="7">
+        <v>17</v>
+      </c>
+      <c r="J119" s="7" t="s">
+        <v>239</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>240</v>
@@ -9211,7 +9523,7 @@
         <v>179</v>
       </c>
       <c r="U119" s="1" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="V119" s="2">
         <v>15.348732999999999</v>
@@ -9220,7 +9532,7 @@
         <v>-88.403704000000005</v>
       </c>
     </row>
-    <row r="120" spans="2:23">
+    <row r="120" spans="2:23" ht="15">
       <c r="B120" s="1" t="s">
         <v>23</v>
       </c>
@@ -9230,17 +9542,26 @@
       <c r="D120" s="1">
         <v>3</v>
       </c>
+      <c r="E120" s="7">
+        <v>7</v>
+      </c>
+      <c r="F120" s="7" t="s">
+        <v>319</v>
+      </c>
       <c r="G120" s="1" t="s">
-        <v>314</v>
+        <v>320</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="S120" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U120" s="1" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="V120" s="2">
         <v>13.861846</v>
@@ -9249,7 +9570,7 @@
         <v>-86.554258000000004</v>
       </c>
     </row>
-    <row r="121" spans="2:23">
+    <row r="121" spans="2:23" ht="15">
       <c r="B121" s="1" t="s">
         <v>23</v>
       </c>
@@ -9259,17 +9580,26 @@
       <c r="D121" s="1">
         <v>3</v>
       </c>
+      <c r="E121" s="7">
+        <v>7</v>
+      </c>
+      <c r="F121" s="7" t="s">
+        <v>319</v>
+      </c>
       <c r="G121" s="1" t="s">
-        <v>314</v>
+        <v>320</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="S121" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U121" s="1" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="V121" s="2">
         <v>13.865371</v>
@@ -9278,7 +9608,7 @@
         <v>-86.562415000000001</v>
       </c>
     </row>
-    <row r="122" spans="2:23">
+    <row r="122" spans="2:23" ht="15">
       <c r="B122" s="1" t="s">
         <v>23</v>
       </c>
@@ -9288,14 +9618,23 @@
       <c r="D122" s="1">
         <v>3</v>
       </c>
+      <c r="E122" s="7">
+        <v>18</v>
+      </c>
+      <c r="F122" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="G122" s="1" t="s">
-        <v>317</v>
+        <v>323</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="S122" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U122" s="1" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="V122" s="2">
         <v>14.985823</v>
@@ -9304,7 +9643,7 @@
         <v>-87.294527000000002</v>
       </c>
     </row>
-    <row r="123" spans="2:23">
+    <row r="123" spans="2:23" ht="15">
       <c r="B123" s="1" t="s">
         <v>23</v>
       </c>
@@ -9313,18 +9652,33 @@
       </c>
       <c r="D123" s="1">
         <v>3</v>
+      </c>
+      <c r="E123" s="7">
+        <v>18</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="H123" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I123" s="8">
+        <v>11</v>
+      </c>
+      <c r="J123" s="8" t="s">
+        <v>325</v>
+      </c>
       <c r="K123" s="1" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="S123" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U123" s="1" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="V123" s="2">
         <v>15.065429</v>
@@ -9343,14 +9697,23 @@
       <c r="D124" s="1">
         <v>3</v>
       </c>
+      <c r="E124" s="7">
+        <v>18</v>
+      </c>
+      <c r="F124" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="G124" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="H124" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="S124" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="V124" s="2">
         <v>15.108616</v>
@@ -9359,7 +9722,7 @@
         <v>-87.280530999999996</v>
       </c>
     </row>
-    <row r="125" spans="2:23">
+    <row r="125" spans="2:23" ht="15">
       <c r="B125" s="1" t="s">
         <v>23</v>
       </c>
@@ -9368,10 +9731,25 @@
       </c>
       <c r="D125" s="1">
         <v>3</v>
+      </c>
+      <c r="E125" s="7">
+        <v>18</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="H125" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I125" s="7">
+        <v>1</v>
+      </c>
+      <c r="J125" s="7" t="s">
+        <v>329</v>
+      </c>
       <c r="K125" s="1" t="s">
         <v>162</v>
       </c>
@@ -9379,7 +9757,7 @@
         <v>72</v>
       </c>
       <c r="U125" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="V125" s="2">
         <v>15.137855999999999</v>
@@ -9388,7 +9766,7 @@
         <v>-87.125667000000007</v>
       </c>
     </row>
-    <row r="126" spans="2:23">
+    <row r="126" spans="2:23" ht="15">
       <c r="B126" s="1" t="s">
         <v>23</v>
       </c>
@@ -9397,10 +9775,25 @@
       </c>
       <c r="D126" s="1">
         <v>3</v>
+      </c>
+      <c r="E126" s="7">
+        <v>18</v>
+      </c>
+      <c r="F126" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="H126" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I126" s="7">
+        <v>1</v>
+      </c>
+      <c r="J126" s="7" t="s">
+        <v>329</v>
+      </c>
       <c r="K126" s="1" t="s">
         <v>162</v>
       </c>
@@ -9408,7 +9801,7 @@
         <v>179</v>
       </c>
       <c r="U126" s="1" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="V126" s="2">
         <v>15.137337</v>
@@ -9427,17 +9820,23 @@
       <c r="D127" s="1">
         <v>3</v>
       </c>
+      <c r="E127" s="7">
+        <v>18</v>
+      </c>
+      <c r="F127" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="G127" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="K127" s="1" t="s">
-        <v>324</v>
+      <c r="H127" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="S127" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U127" s="1" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="V127" s="2">
         <v>15.276194</v>
@@ -9446,7 +9845,7 @@
         <v>-87.324967999999998</v>
       </c>
     </row>
-    <row r="128" spans="2:23">
+    <row r="128" spans="2:23" ht="15">
       <c r="B128" s="1" t="s">
         <v>23</v>
       </c>
@@ -9455,18 +9854,33 @@
       </c>
       <c r="D128" s="1">
         <v>3</v>
+      </c>
+      <c r="E128" s="7">
+        <v>13</v>
+      </c>
+      <c r="F128" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="H128" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I128" s="7">
+        <v>13</v>
+      </c>
+      <c r="J128" s="7" t="s">
+        <v>333</v>
+      </c>
       <c r="K128" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="S128" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="V128" s="2">
         <v>14.780340000000001</v>
@@ -9475,7 +9889,7 @@
         <v>-88.588606999999996</v>
       </c>
     </row>
-    <row r="129" spans="2:23">
+    <row r="129" spans="2:23" ht="15">
       <c r="B129" s="1" t="s">
         <v>23</v>
       </c>
@@ -9484,18 +9898,33 @@
       </c>
       <c r="D129" s="1">
         <v>3</v>
+      </c>
+      <c r="E129" s="7">
+        <v>13</v>
+      </c>
+      <c r="F129" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="H129" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I129" s="7">
+        <v>22</v>
+      </c>
+      <c r="J129" s="7" t="s">
+        <v>336</v>
+      </c>
       <c r="K129" s="1" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="S129" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="V129" s="2">
         <v>14.329539</v>
@@ -9504,7 +9933,7 @@
         <v>-88.522634999999994</v>
       </c>
     </row>
-    <row r="130" spans="2:23">
+    <row r="130" spans="2:23" ht="15">
       <c r="B130" s="1" t="s">
         <v>23</v>
       </c>
@@ -9513,18 +9942,33 @@
       </c>
       <c r="D130" s="1">
         <v>3</v>
+      </c>
+      <c r="E130" s="7">
+        <v>13</v>
+      </c>
+      <c r="F130" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="H130" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I130" s="7">
+        <v>6</v>
+      </c>
+      <c r="J130" s="7" t="s">
+        <v>339</v>
+      </c>
       <c r="K130" s="1" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="S130" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="V130" s="2">
         <v>14.126211</v>
@@ -9543,9 +9987,18 @@
       <c r="D131" s="1">
         <v>3</v>
       </c>
+      <c r="E131" s="7">
+        <v>13</v>
+      </c>
+      <c r="F131" s="7" t="s">
+        <v>142</v>
+      </c>
       <c r="G131" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="H131" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="S131" s="1" t="s">
         <v>36</v>
       </c>
@@ -9559,7 +10012,7 @@
         <v>-88.651722000000007</v>
       </c>
     </row>
-    <row r="132" spans="2:23">
+    <row r="132" spans="2:23" ht="15">
       <c r="B132" s="1" t="s">
         <v>23</v>
       </c>
@@ -9568,18 +10021,33 @@
       </c>
       <c r="D132" s="1">
         <v>3</v>
+      </c>
+      <c r="E132" s="7">
+        <v>17</v>
+      </c>
+      <c r="F132" s="7" t="s">
+        <v>342</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="H132" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I132" s="7">
+        <v>1</v>
+      </c>
+      <c r="J132" s="7" t="s">
+        <v>343</v>
+      </c>
       <c r="K132" s="1" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="S132" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U132" s="1" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="V132" s="2">
         <v>13.530787999999999</v>
@@ -9588,7 +10056,7 @@
         <v>-87.498217999999994</v>
       </c>
     </row>
-    <row r="133" spans="2:23">
+    <row r="133" spans="2:23" ht="15">
       <c r="B133" s="1" t="s">
         <v>23</v>
       </c>
@@ -9597,18 +10065,33 @@
       </c>
       <c r="D133" s="1">
         <v>3</v>
+      </c>
+      <c r="E133" s="7">
+        <v>17</v>
+      </c>
+      <c r="F133" s="7" t="s">
+        <v>342</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="H133" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I133" s="7">
+        <v>1</v>
+      </c>
+      <c r="J133" s="7" t="s">
+        <v>343</v>
+      </c>
       <c r="K133" s="1" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="S133" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U133" s="1" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="V133" s="2">
         <v>13.532709000000001</v>
@@ -9617,7 +10100,7 @@
         <v>-87.492543999999995</v>
       </c>
     </row>
-    <row r="134" spans="2:23">
+    <row r="134" spans="2:23" ht="15">
       <c r="B134" s="1" t="s">
         <v>23</v>
       </c>
@@ -9626,18 +10109,33 @@
       </c>
       <c r="D134" s="1">
         <v>3</v>
+      </c>
+      <c r="E134" s="7">
+        <v>17</v>
+      </c>
+      <c r="F134" s="7" t="s">
+        <v>342</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="H134" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I134" s="7">
+        <v>7</v>
+      </c>
+      <c r="J134" s="7" t="s">
+        <v>347</v>
+      </c>
       <c r="K134" s="1" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="S134" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U134" s="1" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="V134" s="2">
         <v>13.62003</v>
@@ -9646,7 +10144,7 @@
         <v>-87.657388999999995</v>
       </c>
     </row>
-    <row r="135" spans="2:23">
+    <row r="135" spans="2:23" ht="15">
       <c r="B135" s="1" t="s">
         <v>23</v>
       </c>
@@ -9655,18 +10153,33 @@
       </c>
       <c r="D135" s="1">
         <v>3</v>
+      </c>
+      <c r="E135" s="7">
+        <v>17</v>
+      </c>
+      <c r="F135" s="7" t="s">
+        <v>342</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="H135" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I135" s="7">
+        <v>6</v>
+      </c>
+      <c r="J135" s="7" t="s">
+        <v>350</v>
+      </c>
       <c r="K135" s="1" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="S135" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U135" s="1" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
       <c r="V135" s="2">
         <v>13.610545</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-10-2020 04-36-55
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="723" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{529982E2-1FFC-4553-902F-04259DCB81D4}"/>
+  <xr:revisionPtr revIDLastSave="740" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A97B96DF-7FB2-400F-8A27-7A04074535CF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="362">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -882,6 +882,9 @@
     <t>Gracias a Dios</t>
   </si>
   <si>
+    <t>0901</t>
+  </si>
+  <si>
     <t xml:space="preserve">Puerto Lempira </t>
   </si>
   <si>
@@ -912,6 +915,9 @@
     <t>Clínica Medicentro</t>
   </si>
   <si>
+    <t>1206</t>
+  </si>
+  <si>
     <t>Guajiquiro</t>
   </si>
   <si>
@@ -921,21 +927,33 @@
     <t>Centro de Salud El Guajiquiro</t>
   </si>
   <si>
+    <t>1208</t>
+  </si>
+  <si>
     <t>Marcala</t>
   </si>
   <si>
     <t>Centro de Salud Marcala</t>
   </si>
   <si>
+    <t>1212</t>
+  </si>
+  <si>
     <t>San José</t>
   </si>
   <si>
+    <t>1201</t>
+  </si>
+  <si>
     <t>Hospital Montecillos</t>
   </si>
   <si>
     <t>Hospital Roberto Suazo Córdova</t>
   </si>
   <si>
+    <t>0301</t>
+  </si>
+  <si>
     <t>Hospital Regional Santa Teresa</t>
   </si>
   <si>
@@ -945,12 +963,18 @@
     <t>Hospital Privado de Comayagua</t>
   </si>
   <si>
+    <t>1001</t>
+  </si>
+  <si>
     <t>La Esperanza</t>
   </si>
   <si>
     <t>Hospital Enrique Aguila Cerrato</t>
   </si>
   <si>
+    <t>0107</t>
+  </si>
+  <si>
     <t>Tela</t>
   </si>
   <si>
@@ -997,6 +1021,9 @@
   </si>
   <si>
     <t>El Paraíso</t>
+  </si>
+  <si>
+    <t>0704</t>
   </si>
   <si>
     <t>Centro Médico San Francisco</t>
@@ -2091,8 +2118,8 @@
   <dimension ref="A1:W135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="F114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I120" sqref="I120"/>
+      <pane ySplit="1" topLeftCell="D106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J114" sqref="J114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -8632,14 +8659,20 @@
       <c r="H97" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I97" s="7">
+        <v>1</v>
+      </c>
+      <c r="J97" s="7" t="s">
+        <v>282</v>
+      </c>
       <c r="K97" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="S97" s="1" t="s">
         <v>246</v>
       </c>
       <c r="U97" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="V97" s="2">
         <v>15.265726000000001</v>
@@ -8674,16 +8707,16 @@
         <v>1</v>
       </c>
       <c r="J98" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="S98" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U98" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="V98" s="2">
         <v>14.665319</v>
@@ -8718,16 +8751,16 @@
         <v>1</v>
       </c>
       <c r="J99" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="S99" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U99" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="V99" s="2">
         <v>14.671486</v>
@@ -8762,16 +8795,16 @@
         <v>3</v>
       </c>
       <c r="J100" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="S100" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U100" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="V100" s="2">
         <v>14.853908000000001</v>
@@ -8806,16 +8839,16 @@
         <v>3</v>
       </c>
       <c r="J101" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="S101" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U101" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="V101" s="2">
         <v>14.851229</v>
@@ -8850,10 +8883,10 @@
         <v>3</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="S102" s="1" t="s">
         <v>72</v>
@@ -8890,14 +8923,20 @@
       <c r="H103" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I103" s="7">
+        <v>6</v>
+      </c>
+      <c r="J103" s="7" t="s">
+        <v>293</v>
+      </c>
       <c r="K103" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="S103" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="U103" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="V103" s="2">
         <v>14.120423000000001</v>
@@ -8928,14 +8967,20 @@
       <c r="H104" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I104" s="7">
+        <v>8</v>
+      </c>
+      <c r="J104" s="7" t="s">
+        <v>297</v>
+      </c>
       <c r="K104" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="S104" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="S104" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="U104" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="V104" s="2">
         <v>14.159074</v>
@@ -8944,7 +8989,7 @@
         <v>-88.036270999999999</v>
       </c>
     </row>
-    <row r="105" spans="2:23">
+    <row r="105" spans="2:23" ht="15">
       <c r="B105" s="1" t="s">
         <v>23</v>
       </c>
@@ -8966,11 +9011,17 @@
       <c r="H105" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I105" s="7">
+        <v>12</v>
+      </c>
+      <c r="J105" s="7" t="s">
+        <v>300</v>
+      </c>
       <c r="K105" s="1" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="S105" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="U105" s="1" t="s">
         <v>44</v>
@@ -8982,7 +9033,7 @@
         <v>-87.959114999999997</v>
       </c>
     </row>
-    <row r="106" spans="2:23">
+    <row r="106" spans="2:23" ht="15">
       <c r="B106" s="1" t="s">
         <v>23</v>
       </c>
@@ -9004,6 +9055,12 @@
       <c r="H106" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I106" s="7">
+        <v>1</v>
+      </c>
+      <c r="J106" s="7" t="s">
+        <v>302</v>
+      </c>
       <c r="K106" s="1" t="s">
         <v>63</v>
       </c>
@@ -9011,7 +9068,7 @@
         <v>179</v>
       </c>
       <c r="U106" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="V106" s="2">
         <v>14.319006</v>
@@ -9020,7 +9077,7 @@
         <v>-87.680940000000007</v>
       </c>
     </row>
-    <row r="107" spans="2:23">
+    <row r="107" spans="2:23" ht="15">
       <c r="B107" s="1" t="s">
         <v>23</v>
       </c>
@@ -9042,6 +9099,12 @@
       <c r="H107" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I107" s="7">
+        <v>1</v>
+      </c>
+      <c r="J107" s="7" t="s">
+        <v>302</v>
+      </c>
       <c r="K107" s="1" t="s">
         <v>63</v>
       </c>
@@ -9049,7 +9112,7 @@
         <v>179</v>
       </c>
       <c r="U107" s="1" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="V107" s="2">
         <v>14.322329999999999</v>
@@ -9080,6 +9143,12 @@
       <c r="H108" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I108" s="7">
+        <v>1</v>
+      </c>
+      <c r="J108" s="7" t="s">
+        <v>305</v>
+      </c>
       <c r="K108" s="1" t="s">
         <v>189</v>
       </c>
@@ -9087,7 +9156,7 @@
         <v>179</v>
       </c>
       <c r="U108" s="1" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="V108" s="2">
         <v>14.453317999999999</v>
@@ -9118,6 +9187,12 @@
       <c r="H109" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I109" s="7">
+        <v>1</v>
+      </c>
+      <c r="J109" s="7" t="s">
+        <v>305</v>
+      </c>
       <c r="K109" s="1" t="s">
         <v>189</v>
       </c>
@@ -9125,7 +9200,7 @@
         <v>179</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="V109" s="2">
         <v>14.456941</v>
@@ -9134,7 +9209,7 @@
         <v>-87.635479000000004</v>
       </c>
     </row>
-    <row r="110" spans="2:23">
+    <row r="110" spans="2:23" ht="15">
       <c r="B110" s="1" t="s">
         <v>23</v>
       </c>
@@ -9156,6 +9231,12 @@
       <c r="H110" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I110" s="7">
+        <v>1</v>
+      </c>
+      <c r="J110" s="7" t="s">
+        <v>305</v>
+      </c>
       <c r="K110" s="1" t="s">
         <v>189</v>
       </c>
@@ -9163,7 +9244,7 @@
         <v>179</v>
       </c>
       <c r="U110" s="1" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="V110" s="2">
         <v>14.460008999999999</v>
@@ -9172,7 +9253,7 @@
         <v>-87.638285999999994</v>
       </c>
     </row>
-    <row r="111" spans="2:23">
+    <row r="111" spans="2:23" ht="15">
       <c r="B111" s="1" t="s">
         <v>23</v>
       </c>
@@ -9194,6 +9275,12 @@
       <c r="H111" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I111" s="7">
+        <v>18</v>
+      </c>
+      <c r="J111" s="7" t="s">
+        <v>190</v>
+      </c>
       <c r="K111" s="1" t="s">
         <v>191</v>
       </c>
@@ -9232,14 +9319,20 @@
       <c r="H112" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I112" s="7">
+        <v>1</v>
+      </c>
+      <c r="J112" s="7" t="s">
+        <v>309</v>
+      </c>
       <c r="K112" s="1" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="S112" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U112" s="1" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="V112" s="2">
         <v>14.314704000000001</v>
@@ -9270,14 +9363,20 @@
       <c r="H113" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I113" s="7">
+        <v>7</v>
+      </c>
+      <c r="J113" s="7" t="s">
+        <v>312</v>
+      </c>
       <c r="K113" s="1" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="S113" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U113" s="1" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="V113" s="2">
         <v>15.754151999999999</v>
@@ -9312,7 +9411,7 @@
         <v>36</v>
       </c>
       <c r="U114" s="1" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="V114" s="2">
         <v>15.908462</v>
@@ -9338,7 +9437,7 @@
         <v>237</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>27</v>
@@ -9347,16 +9446,16 @@
         <v>1</v>
       </c>
       <c r="J115" s="7" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="S115" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U115" s="1" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="V115" s="2">
         <v>14.925007000000001</v>
@@ -9382,7 +9481,7 @@
         <v>237</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>27</v>
@@ -9391,16 +9490,16 @@
         <v>26</v>
       </c>
       <c r="J116" s="7" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="S116" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U116" s="1" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="V116" s="2">
         <v>15.143121000000001</v>
@@ -9426,7 +9525,7 @@
         <v>237</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>27</v>
@@ -9435,7 +9534,7 @@
         <v>179</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="V117" s="2">
         <v>15.247275</v>
@@ -9461,7 +9560,7 @@
         <v>237</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>27</v>
@@ -9470,16 +9569,16 @@
         <v>15</v>
       </c>
       <c r="J118" s="7" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="S118" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U118" s="1" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="V118" s="2">
         <v>15.273072000000001</v>
@@ -9505,7 +9604,7 @@
         <v>237</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>27</v>
@@ -9523,7 +9622,7 @@
         <v>179</v>
       </c>
       <c r="U119" s="1" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="V119" s="2">
         <v>15.348732999999999</v>
@@ -9546,22 +9645,28 @@
         <v>7</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I120" s="7">
+        <v>4</v>
+      </c>
+      <c r="J120" s="7" t="s">
+        <v>329</v>
+      </c>
       <c r="K120" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="S120" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U120" s="1" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="V120" s="2">
         <v>13.861846</v>
@@ -9584,22 +9689,28 @@
         <v>7</v>
       </c>
       <c r="F121" s="7" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I121" s="7">
+        <v>4</v>
+      </c>
+      <c r="J121" s="7" t="s">
+        <v>329</v>
+      </c>
       <c r="K121" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="S121" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U121" s="1" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="V121" s="2">
         <v>13.865371</v>
@@ -9625,7 +9736,7 @@
         <v>161</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>27</v>
@@ -9634,7 +9745,7 @@
         <v>36</v>
       </c>
       <c r="U122" s="1" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="V122" s="2">
         <v>14.985823</v>
@@ -9669,16 +9780,16 @@
         <v>11</v>
       </c>
       <c r="J123" s="8" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="S123" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U123" s="1" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="V123" s="2">
         <v>15.065429</v>
@@ -9713,7 +9824,7 @@
         <v>36</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="V124" s="2">
         <v>15.108616</v>
@@ -9748,7 +9859,7 @@
         <v>1</v>
       </c>
       <c r="J125" s="7" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="K125" s="1" t="s">
         <v>162</v>
@@ -9757,7 +9868,7 @@
         <v>72</v>
       </c>
       <c r="U125" s="1" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="V125" s="2">
         <v>15.137855999999999</v>
@@ -9792,7 +9903,7 @@
         <v>1</v>
       </c>
       <c r="J126" s="7" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="K126" s="1" t="s">
         <v>162</v>
@@ -9801,7 +9912,7 @@
         <v>179</v>
       </c>
       <c r="U126" s="1" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="V126" s="2">
         <v>15.137337</v>
@@ -9836,7 +9947,7 @@
         <v>72</v>
       </c>
       <c r="U127" s="1" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="V127" s="2">
         <v>15.276194</v>
@@ -9871,16 +9982,16 @@
         <v>13</v>
       </c>
       <c r="J128" s="7" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="S128" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="V128" s="2">
         <v>14.780340000000001</v>
@@ -9915,16 +10026,16 @@
         <v>22</v>
       </c>
       <c r="J129" s="7" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="S129" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="V129" s="2">
         <v>14.329539</v>
@@ -9959,16 +10070,16 @@
         <v>6</v>
       </c>
       <c r="J130" s="7" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="S130" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="V130" s="2">
         <v>14.126211</v>
@@ -10026,7 +10137,7 @@
         <v>17</v>
       </c>
       <c r="F132" s="7" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>275</v>
@@ -10038,16 +10149,16 @@
         <v>1</v>
       </c>
       <c r="J132" s="7" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="S132" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U132" s="1" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="V132" s="2">
         <v>13.530787999999999</v>
@@ -10070,7 +10181,7 @@
         <v>17</v>
       </c>
       <c r="F133" s="7" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>275</v>
@@ -10082,16 +10193,16 @@
         <v>1</v>
       </c>
       <c r="J133" s="7" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="S133" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U133" s="1" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="V133" s="2">
         <v>13.532709000000001</v>
@@ -10114,7 +10225,7 @@
         <v>17</v>
       </c>
       <c r="F134" s="7" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>275</v>
@@ -10126,16 +10237,16 @@
         <v>7</v>
       </c>
       <c r="J134" s="7" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="S134" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U134" s="1" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="V134" s="2">
         <v>13.62003</v>
@@ -10158,7 +10269,7 @@
         <v>17</v>
       </c>
       <c r="F135" s="7" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>275</v>
@@ -10170,16 +10281,16 @@
         <v>6</v>
       </c>
       <c r="J135" s="7" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="S135" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U135" s="1" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="V135" s="2">
         <v>13.610545</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-11-2020 17-39-42
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="740" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A97B96DF-7FB2-400F-8A27-7A04074535CF}"/>
+  <xr:revisionPtr revIDLastSave="756" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{79201995-0D06-4727-B7F9-DF366F1F47F5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="362">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -786,6 +786,9 @@
     <t>Hospital General San Felipe</t>
   </si>
   <si>
+    <t>07</t>
+  </si>
+  <si>
     <t>El Paraiso</t>
   </si>
   <si>
@@ -861,6 +864,9 @@
     <t>Hospital San Marcos de Ocotepeque</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>Valle</t>
   </si>
   <si>
@@ -1017,9 +1023,6 @@
     <t>Centro Médico Integral de Occidente</t>
   </si>
   <si>
-    <t>07</t>
-  </si>
-  <si>
     <t>El Paraíso</t>
   </si>
   <si>
@@ -1087,9 +1090,6 @@
   </si>
   <si>
     <t>Hospital del Sur Dr. Lempira</t>
-  </si>
-  <si>
-    <t>17</t>
   </si>
   <si>
     <t>1701</t>
@@ -2118,8 +2118,8 @@
   <dimension ref="A1:W135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="D106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J114" sqref="J114"/>
+      <pane ySplit="1" topLeftCell="L2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86:F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -2138,7 +2138,7 @@
     <col min="12" max="12" width="12.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="15.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="20.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="15" style="1" customWidth="1"/>
     <col min="18" max="18" width="17.140625" style="1" customWidth="1"/>
@@ -7808,8 +7808,8 @@
       <c r="E84" s="1">
         <v>8</v>
       </c>
-      <c r="F84" s="1">
-        <v>8</v>
+      <c r="F84" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>39</v>
@@ -7876,8 +7876,8 @@
       <c r="E85" s="1">
         <v>8</v>
       </c>
-      <c r="F85" s="1">
-        <v>8</v>
+      <c r="F85" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>39</v>
@@ -7941,14 +7941,14 @@
       <c r="D86" s="1">
         <v>3</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E86" s="7">
         <v>7</v>
       </c>
-      <c r="F86" s="1">
-        <v>7</v>
+      <c r="F86" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>27</v>
@@ -7957,22 +7957,22 @@
         <v>3</v>
       </c>
       <c r="J86" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L86" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O86" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="P86" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q86" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="R86" s="1" t="s">
         <v>35</v>
@@ -7984,7 +7984,7 @@
         <v>247</v>
       </c>
       <c r="U86" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="V86" s="2">
         <v>13.991413</v>
@@ -8006,8 +8006,8 @@
       <c r="E87" s="1">
         <v>11</v>
       </c>
-      <c r="F87" s="1">
-        <v>11</v>
+      <c r="F87" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>56</v>
@@ -8046,7 +8046,7 @@
         <v>247</v>
       </c>
       <c r="U87" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="V87" s="2">
         <v>16.317903000000001</v>
@@ -8068,8 +8068,8 @@
       <c r="E88" s="1">
         <v>5</v>
       </c>
-      <c r="F88" s="1">
-        <v>5</v>
+      <c r="F88" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>85</v>
@@ -8114,7 +8114,7 @@
         <v>247</v>
       </c>
       <c r="U88" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="V88" s="2">
         <v>15.524452999999999</v>
@@ -8136,8 +8136,8 @@
       <c r="E89" s="1">
         <v>5</v>
       </c>
-      <c r="F89" s="1">
-        <v>5</v>
+      <c r="F89" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>85</v>
@@ -8182,7 +8182,7 @@
         <v>247</v>
       </c>
       <c r="U89" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="V89" s="2">
         <v>15.500176</v>
@@ -8204,8 +8204,8 @@
       <c r="E90" s="1">
         <v>5</v>
       </c>
-      <c r="F90" s="1">
-        <v>5</v>
+      <c r="F90" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>85</v>
@@ -8220,7 +8220,7 @@
         <v>92</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L90" s="1" t="s">
         <v>30</v>
@@ -8232,7 +8232,7 @@
         <v>94</v>
       </c>
       <c r="O90" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="P90" s="1" t="s">
         <v>33</v>
@@ -8250,7 +8250,7 @@
         <v>247</v>
       </c>
       <c r="U90" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="V90" s="2">
         <v>15.814730000000001</v>
@@ -8272,8 +8272,8 @@
       <c r="E91" s="1">
         <v>6</v>
       </c>
-      <c r="F91" s="1">
-        <v>6</v>
+      <c r="F91" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>98</v>
@@ -8318,7 +8318,7 @@
         <v>247</v>
       </c>
       <c r="U91" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="V91" s="2">
         <v>13.303027999999999</v>
@@ -8340,8 +8340,8 @@
       <c r="E92" s="1">
         <v>1</v>
       </c>
-      <c r="F92" s="1">
-        <v>1</v>
+      <c r="F92" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>26</v>
@@ -8380,7 +8380,7 @@
         <v>247</v>
       </c>
       <c r="U92" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="V92" s="2">
         <v>15.769266</v>
@@ -8415,22 +8415,22 @@
         <v>1</v>
       </c>
       <c r="J93" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L93" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O93" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="P93" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q93" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="R93" s="1" t="s">
         <v>35</v>
@@ -8442,7 +8442,7 @@
         <v>247</v>
       </c>
       <c r="U93" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="V93" s="2">
         <v>14.768719000000001</v>
@@ -8477,22 +8477,22 @@
         <v>1</v>
       </c>
       <c r="J94" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L94" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O94" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P94" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q94" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="R94" s="1" t="s">
         <v>35</v>
@@ -8504,7 +8504,7 @@
         <v>247</v>
       </c>
       <c r="U94" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="V94" s="2">
         <v>15.920894000000001</v>
@@ -8530,7 +8530,7 @@
         <v>14</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>27</v>
@@ -8539,22 +8539,22 @@
         <v>13</v>
       </c>
       <c r="J95" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L95" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O95" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="P95" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q95" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="R95" s="1" t="s">
         <v>35</v>
@@ -8566,7 +8566,7 @@
         <v>247</v>
       </c>
       <c r="U95" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="V95" s="2">
         <v>14.412167999999999</v>
@@ -8585,14 +8585,14 @@
       <c r="D96" s="1">
         <v>3</v>
       </c>
-      <c r="E96" s="1">
+      <c r="E96" s="7">
         <v>17</v>
       </c>
-      <c r="F96" s="1">
-        <v>17</v>
+      <c r="F96" s="7" t="s">
+        <v>276</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>27</v>
@@ -8601,22 +8601,22 @@
         <v>9</v>
       </c>
       <c r="J96" s="7" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="L96" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O96" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="P96" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q96" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="R96" s="1" t="s">
         <v>35</v>
@@ -8628,7 +8628,7 @@
         <v>247</v>
       </c>
       <c r="U96" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="V96" s="2">
         <v>13.435276</v>
@@ -8651,10 +8651,10 @@
         <v>9</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>27</v>
@@ -8663,16 +8663,19 @@
         <v>1</v>
       </c>
       <c r="J97" s="7" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S97" s="1" t="s">
         <v>246</v>
       </c>
       <c r="U97" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="V97" s="2">
         <v>15.265726000000001</v>
@@ -8707,16 +8710,19 @@
         <v>1</v>
       </c>
       <c r="J98" s="7" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S98" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U98" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="V98" s="2">
         <v>14.665319</v>
@@ -8751,16 +8757,19 @@
         <v>1</v>
       </c>
       <c r="J99" s="7" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S99" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U99" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="V99" s="2">
         <v>14.671486</v>
@@ -8795,16 +8804,19 @@
         <v>3</v>
       </c>
       <c r="J100" s="7" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
+      </c>
+      <c r="L100" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S100" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U100" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="V100" s="2">
         <v>14.853908000000001</v>
@@ -8839,16 +8851,19 @@
         <v>3</v>
       </c>
       <c r="J101" s="7" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
+      </c>
+      <c r="L101" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S101" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U101" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="V101" s="2">
         <v>14.851229</v>
@@ -8883,10 +8898,13 @@
         <v>3</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S102" s="1" t="s">
         <v>72</v>
@@ -8927,16 +8945,19 @@
         <v>6</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
+      </c>
+      <c r="L103" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S103" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="U103" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="V103" s="2">
         <v>14.120423000000001</v>
@@ -8971,16 +8992,19 @@
         <v>8</v>
       </c>
       <c r="J104" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="L104" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S104" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="K104" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="S104" s="1" t="s">
-        <v>295</v>
-      </c>
       <c r="U104" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="V104" s="2">
         <v>14.159074</v>
@@ -9015,13 +9039,16 @@
         <v>12</v>
       </c>
       <c r="J105" s="7" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S105" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="U105" s="1" t="s">
         <v>44</v>
@@ -9059,16 +9086,19 @@
         <v>1</v>
       </c>
       <c r="J106" s="7" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="L106" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S106" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U106" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="V106" s="2">
         <v>14.319006</v>
@@ -9103,16 +9133,19 @@
         <v>1</v>
       </c>
       <c r="J107" s="7" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="L107" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S107" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U107" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="V107" s="2">
         <v>14.322329999999999</v>
@@ -9147,16 +9180,19 @@
         <v>1</v>
       </c>
       <c r="J108" s="7" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="K108" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="L108" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S108" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U108" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="V108" s="2">
         <v>14.453317999999999</v>
@@ -9191,16 +9227,19 @@
         <v>1</v>
       </c>
       <c r="J109" s="7" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="K109" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="L109" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S109" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="V109" s="2">
         <v>14.456941</v>
@@ -9235,16 +9274,19 @@
         <v>1</v>
       </c>
       <c r="J110" s="7" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="L110" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S110" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U110" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="V110" s="2">
         <v>14.460008999999999</v>
@@ -9284,6 +9326,9 @@
       <c r="K111" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="L111" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S111" s="1" t="s">
         <v>179</v>
       </c>
@@ -9323,16 +9368,19 @@
         <v>1</v>
       </c>
       <c r="J112" s="7" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
+      </c>
+      <c r="L112" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S112" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U112" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="V112" s="2">
         <v>14.314704000000001</v>
@@ -9367,16 +9415,19 @@
         <v>7</v>
       </c>
       <c r="J113" s="7" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
+      </c>
+      <c r="L113" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S113" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U113" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="V113" s="2">
         <v>15.754151999999999</v>
@@ -9399,19 +9450,22 @@
         <v>9</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="L114" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S114" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U114" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="V114" s="2">
         <v>15.908462</v>
@@ -9437,7 +9491,7 @@
         <v>237</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>27</v>
@@ -9446,16 +9500,19 @@
         <v>1</v>
       </c>
       <c r="J115" s="7" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
+      </c>
+      <c r="L115" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S115" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U115" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="V115" s="2">
         <v>14.925007000000001</v>
@@ -9481,7 +9538,7 @@
         <v>237</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>27</v>
@@ -9490,16 +9547,19 @@
         <v>26</v>
       </c>
       <c r="J116" s="7" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
+      </c>
+      <c r="L116" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S116" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U116" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="V116" s="2">
         <v>15.143121000000001</v>
@@ -9525,16 +9585,19 @@
         <v>237</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="L117" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S117" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="V117" s="2">
         <v>15.247275</v>
@@ -9560,7 +9623,7 @@
         <v>237</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>27</v>
@@ -9569,16 +9632,19 @@
         <v>15</v>
       </c>
       <c r="J118" s="7" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S118" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U118" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="V118" s="2">
         <v>15.273072000000001</v>
@@ -9604,7 +9670,7 @@
         <v>237</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>27</v>
@@ -9618,11 +9684,14 @@
       <c r="K119" s="1" t="s">
         <v>240</v>
       </c>
+      <c r="L119" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S119" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U119" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="V119" s="2">
         <v>15.348732999999999</v>
@@ -9645,10 +9714,10 @@
         <v>7</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>327</v>
+        <v>250</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>27</v>
@@ -9657,16 +9726,19 @@
         <v>4</v>
       </c>
       <c r="J120" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="K120" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="K120" s="1" t="s">
-        <v>328</v>
+      <c r="L120" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S120" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U120" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="V120" s="2">
         <v>13.861846</v>
@@ -9689,10 +9761,10 @@
         <v>7</v>
       </c>
       <c r="F121" s="7" t="s">
-        <v>327</v>
+        <v>250</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>27</v>
@@ -9701,16 +9773,19 @@
         <v>4</v>
       </c>
       <c r="J121" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="K121" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="K121" s="1" t="s">
-        <v>328</v>
+      <c r="L121" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S121" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U121" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="V121" s="2">
         <v>13.865371</v>
@@ -9736,16 +9811,19 @@
         <v>161</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="L122" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S122" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U122" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="V122" s="2">
         <v>14.985823</v>
@@ -9780,16 +9858,19 @@
         <v>11</v>
       </c>
       <c r="J123" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
+      </c>
+      <c r="L123" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S123" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U123" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="V123" s="2">
         <v>15.065429</v>
@@ -9820,11 +9901,14 @@
       <c r="H124" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="L124" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S124" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="V124" s="2">
         <v>15.108616</v>
@@ -9859,16 +9943,19 @@
         <v>1</v>
       </c>
       <c r="J125" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K125" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="L125" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S125" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U125" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="V125" s="2">
         <v>15.137855999999999</v>
@@ -9903,16 +9990,19 @@
         <v>1</v>
       </c>
       <c r="J126" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K126" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="L126" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S126" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U126" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="V126" s="2">
         <v>15.137337</v>
@@ -9943,11 +10033,14 @@
       <c r="H127" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="L127" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S127" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U127" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="V127" s="2">
         <v>15.276194</v>
@@ -9982,16 +10075,19 @@
         <v>13</v>
       </c>
       <c r="J128" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
+      </c>
+      <c r="L128" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S128" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="V128" s="2">
         <v>14.780340000000001</v>
@@ -10026,16 +10122,19 @@
         <v>22</v>
       </c>
       <c r="J129" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S129" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="V129" s="2">
         <v>14.329539</v>
@@ -10070,16 +10169,19 @@
         <v>6</v>
       </c>
       <c r="J130" s="7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
+      </c>
+      <c r="L130" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S130" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="V130" s="2">
         <v>14.126211</v>
@@ -10110,6 +10212,9 @@
       <c r="H131" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="L131" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S131" s="1" t="s">
         <v>36</v>
       </c>
@@ -10137,10 +10242,10 @@
         <v>17</v>
       </c>
       <c r="F132" s="7" t="s">
-        <v>351</v>
+        <v>276</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>27</v>
@@ -10154,6 +10259,9 @@
       <c r="K132" s="1" t="s">
         <v>353</v>
       </c>
+      <c r="L132" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S132" s="1" t="s">
         <v>72</v>
       </c>
@@ -10181,10 +10289,10 @@
         <v>17</v>
       </c>
       <c r="F133" s="7" t="s">
-        <v>351</v>
+        <v>276</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H133" s="1" t="s">
         <v>27</v>
@@ -10198,6 +10306,9 @@
       <c r="K133" s="1" t="s">
         <v>353</v>
       </c>
+      <c r="L133" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S133" s="1" t="s">
         <v>179</v>
       </c>
@@ -10225,10 +10336,10 @@
         <v>17</v>
       </c>
       <c r="F134" s="7" t="s">
-        <v>351</v>
+        <v>276</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>27</v>
@@ -10242,6 +10353,9 @@
       <c r="K134" s="1" t="s">
         <v>357</v>
       </c>
+      <c r="L134" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S134" s="1" t="s">
         <v>36</v>
       </c>
@@ -10269,10 +10383,10 @@
         <v>17</v>
       </c>
       <c r="F135" s="7" t="s">
-        <v>351</v>
+        <v>276</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H135" s="1" t="s">
         <v>27</v>
@@ -10285,6 +10399,9 @@
       </c>
       <c r="K135" s="1" t="s">
         <v>360</v>
+      </c>
+      <c r="L135" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S135" s="1" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-12-2020 15-04-46
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1195" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3A83A47F-7C1E-4275-9EE0-F26CB5F2BF34}"/>
+  <xr:revisionPtr revIDLastSave="1357" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A188120A-4053-41D4-8566-701DDE9CB935}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="HOSPITALES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$161</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$173</definedName>
     <definedName name="_xlnm.Database">HOSPITALES!$A$1:$U$83</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2234" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2406" uniqueCount="490">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -1362,7 +1362,148 @@
     <t>HND-0510</t>
   </si>
   <si>
-    <t>HND-</t>
+    <t>0203</t>
+  </si>
+  <si>
+    <t>Iriona</t>
+  </si>
+  <si>
+    <t>020309</t>
+  </si>
+  <si>
+    <t>Sangrelaya</t>
+  </si>
+  <si>
+    <t>HND-0203</t>
+  </si>
+  <si>
+    <t>0204</t>
+  </si>
+  <si>
+    <t>Limón</t>
+  </si>
+  <si>
+    <t>020401</t>
+  </si>
+  <si>
+    <t>HND-0204</t>
+  </si>
+  <si>
+    <t>0210</t>
+  </si>
+  <si>
+    <t>Bonito Oriental</t>
+  </si>
+  <si>
+    <t>021001</t>
+  </si>
+  <si>
+    <t>HND-0210</t>
+  </si>
+  <si>
+    <t>0205</t>
+  </si>
+  <si>
+    <t>Sabá</t>
+  </si>
+  <si>
+    <t>020511</t>
+  </si>
+  <si>
+    <t>Elixir</t>
+  </si>
+  <si>
+    <t>HND-0205</t>
+  </si>
+  <si>
+    <t>0320</t>
+  </si>
+  <si>
+    <t>Las Lajas</t>
+  </si>
+  <si>
+    <t>032001</t>
+  </si>
+  <si>
+    <t>HND-0320</t>
+  </si>
+  <si>
+    <t>0321</t>
+  </si>
+  <si>
+    <t>Taulabé</t>
+  </si>
+  <si>
+    <t>032101</t>
+  </si>
+  <si>
+    <t>HND-0321</t>
+  </si>
+  <si>
+    <t>0303</t>
+  </si>
+  <si>
+    <t>El Rosario</t>
+  </si>
+  <si>
+    <t>030301</t>
+  </si>
+  <si>
+    <t>HND-0303</t>
+  </si>
+  <si>
+    <t>0319</t>
+  </si>
+  <si>
+    <t>Villa de San Antonio</t>
+  </si>
+  <si>
+    <t>031901</t>
+  </si>
+  <si>
+    <t>HND-0319</t>
+  </si>
+  <si>
+    <t>Cucuyagua</t>
+  </si>
+  <si>
+    <t>HND-0406</t>
+  </si>
+  <si>
+    <t>Dulce Nombre</t>
+  </si>
+  <si>
+    <t>HND-0408</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>San Nicolas</t>
+  </si>
+  <si>
+    <t>HND-0419</t>
+  </si>
+  <si>
+    <t>Nueva Arcadia</t>
+  </si>
+  <si>
+    <t>041301</t>
+  </si>
+  <si>
+    <t>La Entrada</t>
+  </si>
+  <si>
+    <t>HND-0413</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>041001</t>
+  </si>
+  <si>
+    <t>HND-0410</t>
   </si>
 </sst>
 </file>
@@ -2032,8 +2173,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W161" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W161" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W173" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W173" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W83">
     <sortCondition ref="S1:S83"/>
   </sortState>
@@ -2363,11 +2504,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W161"/>
+  <dimension ref="A1:W173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="U154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W162" sqref="W162"/>
+      <pane ySplit="1" topLeftCell="U162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W174" sqref="W174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -8653,8 +8794,8 @@
       <c r="E93" s="1">
         <v>4</v>
       </c>
-      <c r="F93" s="11">
-        <v>4</v>
+      <c r="F93" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>78</v>
@@ -12495,7 +12636,7 @@
         <v>-87.890918999999997</v>
       </c>
     </row>
-    <row r="161" spans="2:19">
+    <row r="161" spans="2:23">
       <c r="B161" s="1" t="s">
         <v>23</v>
       </c>
@@ -12505,27 +12646,785 @@
       <c r="D161" s="1">
         <v>3</v>
       </c>
-      <c r="E161" s="7"/>
-      <c r="F161" s="10"/>
+      <c r="E161" s="7">
+        <v>2</v>
+      </c>
+      <c r="F161" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="H161" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J161" s="11"/>
+      <c r="I161" s="1">
+        <v>3</v>
+      </c>
+      <c r="J161" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="K161" s="1" t="s">
+        <v>443</v>
+      </c>
       <c r="L161" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N161" s="11"/>
+      <c r="M161" s="1">
+        <v>9</v>
+      </c>
+      <c r="N161" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="O161" s="1" t="s">
+        <v>445</v>
+      </c>
       <c r="P161" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q161" s="1" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="R161" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S161" s="1" t="s">
         <v>361</v>
+      </c>
+      <c r="V161" s="2">
+        <v>15.966279</v>
+      </c>
+      <c r="W161" s="2">
+        <v>-85.096109999999996</v>
+      </c>
+    </row>
+    <row r="162" spans="2:23">
+      <c r="B162" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D162" s="1">
+        <v>3</v>
+      </c>
+      <c r="E162" s="7">
+        <v>2</v>
+      </c>
+      <c r="F162" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I162" s="1">
+        <v>4</v>
+      </c>
+      <c r="J162" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="K162" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="L162" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M162" s="1">
+        <v>1</v>
+      </c>
+      <c r="N162" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="O162" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="P162" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q162" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="R162" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S162" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V162" s="2">
+        <v>15.864474080000001</v>
+      </c>
+      <c r="W162" s="2">
+        <v>-85.506744999999995</v>
+      </c>
+    </row>
+    <row r="163" spans="2:23">
+      <c r="B163" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D163" s="1">
+        <v>3</v>
+      </c>
+      <c r="E163" s="7">
+        <v>2</v>
+      </c>
+      <c r="F163" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I163" s="1">
+        <v>10</v>
+      </c>
+      <c r="J163" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="K163" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="L163" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M163" s="1">
+        <v>1</v>
+      </c>
+      <c r="N163" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="O163" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="P163" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q163" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="R163" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S163" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V163" s="2">
+        <v>15.748343</v>
+      </c>
+      <c r="W163" s="2">
+        <v>-85.735150000000004</v>
+      </c>
+    </row>
+    <row r="164" spans="2:23">
+      <c r="B164" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D164" s="1">
+        <v>3</v>
+      </c>
+      <c r="E164" s="7">
+        <v>2</v>
+      </c>
+      <c r="F164" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I164" s="1">
+        <v>5</v>
+      </c>
+      <c r="J164" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="K164" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="L164" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M164" s="1">
+        <v>11</v>
+      </c>
+      <c r="N164" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="O164" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="P164" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q164" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="R164" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S164" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V164" s="2">
+        <v>15.534311000000001</v>
+      </c>
+      <c r="W164" s="2">
+        <v>-86.273984999999996</v>
+      </c>
+    </row>
+    <row r="165" spans="2:23">
+      <c r="B165" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D165" s="1">
+        <v>3</v>
+      </c>
+      <c r="E165" s="7">
+        <v>3</v>
+      </c>
+      <c r="F165" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I165" s="1">
+        <v>20</v>
+      </c>
+      <c r="J165" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="K165" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="L165" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M165" s="1">
+        <v>1</v>
+      </c>
+      <c r="N165" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="O165" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="P165" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q165" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="R165" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S165" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V165" s="2">
+        <v>14.894002</v>
+      </c>
+      <c r="W165" s="2">
+        <v>-87.579126000000002</v>
+      </c>
+    </row>
+    <row r="166" spans="2:23">
+      <c r="B166" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D166" s="1">
+        <v>3</v>
+      </c>
+      <c r="E166" s="7">
+        <v>3</v>
+      </c>
+      <c r="F166" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I166" s="1">
+        <v>21</v>
+      </c>
+      <c r="J166" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="K166" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="L166" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M166" s="1">
+        <v>1</v>
+      </c>
+      <c r="N166" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="O166" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="P166" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q166" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="R166" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S166" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V166" s="2">
+        <v>14.690765000000001</v>
+      </c>
+      <c r="W166" s="2">
+        <v>-87.965248000000003</v>
+      </c>
+    </row>
+    <row r="167" spans="2:23">
+      <c r="B167" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D167" s="1">
+        <v>3</v>
+      </c>
+      <c r="E167" s="7">
+        <v>3</v>
+      </c>
+      <c r="F167" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I167" s="1">
+        <v>3</v>
+      </c>
+      <c r="J167" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="K167" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="L167" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M167" s="1">
+        <v>1</v>
+      </c>
+      <c r="N167" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="O167" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="P167" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q167" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="R167" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S167" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V167" s="2">
+        <v>14.575887</v>
+      </c>
+      <c r="W167" s="2">
+        <v>-87.728960000000001</v>
+      </c>
+    </row>
+    <row r="168" spans="2:23">
+      <c r="B168" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D168" s="1">
+        <v>3</v>
+      </c>
+      <c r="E168" s="7">
+        <v>3</v>
+      </c>
+      <c r="F168" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I168" s="1">
+        <v>19</v>
+      </c>
+      <c r="J168" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="K168" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="L168" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M168" s="1">
+        <v>1</v>
+      </c>
+      <c r="N168" s="11" t="s">
+        <v>474</v>
+      </c>
+      <c r="O168" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="P168" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q168" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="R168" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S168" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V168" s="2">
+        <v>14.323912999999999</v>
+      </c>
+      <c r="W168" s="2">
+        <v>-87.613690000000005</v>
+      </c>
+    </row>
+    <row r="169" spans="2:23">
+      <c r="B169" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D169" s="1">
+        <v>3</v>
+      </c>
+      <c r="E169" s="7">
+        <v>4</v>
+      </c>
+      <c r="F169" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I169" s="1">
+        <v>6</v>
+      </c>
+      <c r="J169" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="K169" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="L169" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N169" s="11"/>
+      <c r="O169" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="P169" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q169" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="R169" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S169" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V169" s="2">
+        <v>14.645818</v>
+      </c>
+      <c r="W169" s="2">
+        <v>-88.873898999999994</v>
+      </c>
+    </row>
+    <row r="170" spans="2:23">
+      <c r="B170" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D170" s="1">
+        <v>3</v>
+      </c>
+      <c r="E170" s="7">
+        <v>4</v>
+      </c>
+      <c r="F170" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I170" s="1">
+        <v>8</v>
+      </c>
+      <c r="J170" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K170" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="L170" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N170" s="11"/>
+      <c r="O170" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="P170" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q170" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="R170" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S170" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V170" s="2">
+        <v>14.845943</v>
+      </c>
+      <c r="W170" s="2">
+        <v>-88.831519999999998</v>
+      </c>
+    </row>
+    <row r="171" spans="2:23">
+      <c r="B171" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D171" s="1">
+        <v>3</v>
+      </c>
+      <c r="E171" s="7">
+        <v>4</v>
+      </c>
+      <c r="F171" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I171" s="1">
+        <v>19</v>
+      </c>
+      <c r="J171" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="K171" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="L171" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N171" s="11"/>
+      <c r="O171" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="P171" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q171" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="R171" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S171" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V171" s="2">
+        <v>15.001557999999999</v>
+      </c>
+      <c r="W171" s="2">
+        <v>-88.751771000000005</v>
+      </c>
+    </row>
+    <row r="172" spans="2:23">
+      <c r="B172" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D172" s="1">
+        <v>3</v>
+      </c>
+      <c r="E172" s="7">
+        <v>4</v>
+      </c>
+      <c r="F172" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I172" s="1">
+        <v>13</v>
+      </c>
+      <c r="J172" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K172" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="L172" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M172" s="1">
+        <v>1</v>
+      </c>
+      <c r="N172" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="O172" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="P172" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q172" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="R172" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S172" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V172" s="2">
+        <v>15.061814</v>
+      </c>
+      <c r="W172" s="2">
+        <v>-88.746099000000001</v>
+      </c>
+    </row>
+    <row r="173" spans="2:23">
+      <c r="B173" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D173" s="1">
+        <v>3</v>
+      </c>
+      <c r="E173" s="7">
+        <v>4</v>
+      </c>
+      <c r="F173" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H173" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I173" s="1">
+        <v>10</v>
+      </c>
+      <c r="J173" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="K173" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="L173" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M173" s="1">
+        <v>1</v>
+      </c>
+      <c r="N173" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="O173" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="P173" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q173" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="R173" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S173" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V173" s="2">
+        <v>15.024939</v>
+      </c>
+      <c r="W173" s="2">
+        <v>-88.835689000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>